<commit_message>
Grid and Platypus improvements
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\MaSc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5189AFA4-CCA2-4869-B2D5-A3960B7D1F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4957C998-E2E3-4045-AC9A-71653D105164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
+    <workbookView xWindow="24408" yWindow="-2412" windowWidth="21600" windowHeight="11388" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="115">
   <si>
     <t>File</t>
   </si>
@@ -261,12 +261,6 @@
   </si>
   <si>
     <t>Note: What is interesting from the note on the left is that as I increase pixelDiv, the error seen in the linalg_lu solution is still very low and stays roughly constant meaning that linalg_lu is valid for all but the values being passed in may be garbage</t>
-  </si>
-  <si>
-    <t>Note: Some things I can still try are  checking how I assigned an and bn after solving the matrix. Also I run sims at pixelDiv at 2 but I should go once through it all at Div 4 and make sure it still looks correct. Also what is weird is that the airgap plot looks more correct at Div = 2 than Div = 15 which makes me think there is an error in the mec region. I wonder if this is because of the MMF scaling</t>
-  </si>
-  <si>
-    <t>What I should look into is the MMF scaling again</t>
   </si>
   <si>
     <t>Try different values for pixelDiv and write down all the expected values on the excel sheet like Y_bc and the indexes</t>
@@ -394,6 +388,21 @@
   <si>
     <t xml:space="preserve">I am confident that error is negligible in flux conservation (e-18).
 I am also confident that LU Decomp error is negligibile (e-14) </t>
+  </si>
+  <si>
+    <t>What I don’t understand in the 2019 paper is that phase rotation in + direction is A, C, B</t>
+  </si>
+  <si>
+    <t>One possible thing to try if all else fails is to transpose the coordinate system of tkinter to be normal in case that messed me up somewhere</t>
+  </si>
+  <si>
+    <t>MAKE SURE THE ASSUMPTIONS IN 2019 TABLE 1 MATCH MY STUFF. Document any deviation</t>
+  </si>
+  <si>
+    <t>Note: the airgap plot looks more correct at Div = 2 than Div = 15 which makes me think there is an error in the mec region</t>
+  </si>
+  <si>
+    <t>Something really interesting with the plot of the error of the conservation of flux equation after solving the linear system of equations is that when leaving mmf in an normal state I see max error e^-18 but if I purposfully introduce an error I still see  a really low error like e^-19. this means that an error in MMF early is not caught by this plot. Question is what is this plot used for</t>
   </si>
 </sst>
 </file>
@@ -1853,8 +1862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2247,7 +2256,7 @@
         <v>100</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F16" s="7" t="str">
         <v>LIM_Compute</v>
@@ -2321,7 +2330,7 @@
         <v>100</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F19" s="7" t="str">
         <v>LIM_Compute</v>
@@ -2360,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
@@ -2611,7 +2620,7 @@
         <v>100</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F31" s="7" t="str">
         <v>LIM_Compute</v>
@@ -3269,12 +3278,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="315" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="285" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>67</v>
@@ -3288,20 +3297,29 @@
     </row>
     <row r="60" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D60" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="B62" s="7"/>
+      <c r="C62" s="15" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
@@ -3330,7 +3348,7 @@
   <dimension ref="A1:EB26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3341,7 +3359,7 @@
   <sheetData>
     <row r="1" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B1" s="9">
         <v>12</v>
@@ -3349,13 +3367,13 @@
     </row>
     <row r="2" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="8">
         <v>116</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -3380,13 +3398,13 @@
     </row>
     <row r="3" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" s="8">
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
@@ -3417,7 +3435,7 @@
     </row>
     <row r="4" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" s="8">
         <v>6</v>
@@ -3488,14 +3506,14 @@
     </row>
     <row r="5" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="8">
         <v>1</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F5" s="8">
         <v>3</v>
@@ -3527,14 +3545,14 @@
     </row>
     <row r="6" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="8">
         <v>35</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F6" s="8">
         <v>7</v>
@@ -3574,14 +3592,14 @@
     </row>
     <row r="7" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7" s="8">
         <v>20</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F7" s="8">
         <v>15</v>
@@ -3621,13 +3639,13 @@
     </row>
     <row r="8" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8" s="8">
         <v>432</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E8" s="8">
         <v>23</v>
@@ -3656,13 +3674,13 @@
     </row>
     <row r="9" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" s="8">
         <v>6</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E9" s="8">
         <v>25</v>
@@ -3689,13 +3707,13 @@
     </row>
     <row r="10" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="8">
         <v>432</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E10" s="8">
         <v>26</v>
@@ -3732,13 +3750,13 @@
     </row>
     <row r="11" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" s="8">
         <v>6</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E11" s="8">
         <v>32</v>
@@ -3769,7 +3787,7 @@
     </row>
     <row r="12" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12" s="8">
         <v>8</v>
@@ -3777,13 +3795,13 @@
     </row>
     <row r="13" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B13" s="8">
         <v>16</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E13" s="8">
         <v>122</v>
@@ -4172,13 +4190,13 @@
     </row>
     <row r="14" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B14" s="8">
         <v>12</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E14" s="8">
         <v>116</v>
@@ -4455,7 +4473,7 @@
     </row>
     <row r="15" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B15" s="8">
         <v>4</v>
@@ -4463,7 +4481,7 @@
     </row>
     <row r="16" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B16" s="8">
         <v>3</v>
@@ -4471,7 +4489,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B17" s="8">
         <v>3</v>
@@ -4479,7 +4497,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B18" s="8">
         <v>4</v>
@@ -4487,7 +4505,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B19" s="8">
         <v>16</v>
@@ -4495,7 +4513,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B20" s="8">
         <v>8640</v>
@@ -4503,7 +4521,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B21" s="8">
         <v>100</v>
@@ -4511,22 +4529,22 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the graphics for Field plots
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\MaSc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4957C998-E2E3-4045-AC9A-71653D105164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD292ED-09A1-4A8C-BD18-6BB131E921C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24408" yWindow="-2412" windowWidth="21600" windowHeight="11388" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="2" r:id="rId1"/>
     <sheet name="TrackVars" sheetId="3" r:id="rId2"/>
+    <sheet name="TrackConstants" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="161">
   <si>
     <t>File</t>
   </si>
@@ -396,20 +397,158 @@
     <t>One possible thing to try if all else fails is to transpose the coordinate system of tkinter to be normal in case that messed me up somewhere</t>
   </si>
   <si>
-    <t>MAKE SURE THE ASSUMPTIONS IN 2019 TABLE 1 MATCH MY STUFF. Document any deviation</t>
-  </si>
-  <si>
     <t>Note: the airgap plot looks more correct at Div = 2 than Div = 15 which makes me think there is an error in the mec region</t>
   </si>
   <si>
-    <t>Something really interesting with the plot of the error of the conservation of flux equation after solving the linear system of equations is that when leaving mmf in an normal state I see max error e^-18 but if I purposfully introduce an error I still see  a really low error like e^-19. this means that an error in MMF early is not caught by this plot. Question is what is this plot used for</t>
+    <t>Np</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2p</t>
+  </si>
+  <si>
+    <t>z1</t>
+  </si>
+  <si>
+    <t>Nt</t>
+  </si>
+  <si>
+    <t>Ls</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>ws</t>
+  </si>
+  <si>
+    <t>hs</t>
+  </si>
+  <si>
+    <t>hy</t>
+  </si>
+  <si>
+    <t>hg</t>
+  </si>
+  <si>
+    <t>hAl</t>
+  </si>
+  <si>
+    <t>hbi</t>
+  </si>
+  <si>
+    <t>sAl</t>
+  </si>
+  <si>
+    <t>sFe</t>
+  </si>
+  <si>
+    <t>ur</t>
+  </si>
+  <si>
+    <t>4.5*10^6</t>
+  </si>
+  <si>
+    <t>17*10^6</t>
+  </si>
+  <si>
+    <t>Sm^-1</t>
+  </si>
+  <si>
+    <t>Number of phases</t>
+  </si>
+  <si>
+    <t>Number of poles</t>
+  </si>
+  <si>
+    <t>Number of slots</t>
+  </si>
+  <si>
+    <t>Number of turns per coil</t>
+  </si>
+  <si>
+    <t>Stack width</t>
+  </si>
+  <si>
+    <t>Fundamental pitch of the primary</t>
+  </si>
+  <si>
+    <t>Primary tooth width</t>
+  </si>
+  <si>
+    <t>Primary slot width</t>
+  </si>
+  <si>
+    <t>Primary slot height</t>
+  </si>
+  <si>
+    <t>Primary yoke height</t>
+  </si>
+  <si>
+    <t>Air gap length</t>
+  </si>
+  <si>
+    <t>Thickness of the aluminum plate</t>
+  </si>
+  <si>
+    <t>Thickness of the back-iron plate</t>
+  </si>
+  <si>
+    <t>Conductivity of aluminum</t>
+  </si>
+  <si>
+    <t>Conductivity of iron</t>
+  </si>
+  <si>
+    <t>Relative permeability iron</t>
+  </si>
+  <si>
+    <t>Conductivity of airgap</t>
+  </si>
+  <si>
+    <t>3*10^-15</t>
+  </si>
+  <si>
+    <t>Conductivity of copper</t>
+  </si>
+  <si>
+    <t>5.96*10^6</t>
+  </si>
+  <si>
+    <t>Relative permeability aluminum</t>
+  </si>
+  <si>
+    <t>Relative permeability air</t>
+  </si>
+  <si>
+    <t>Relative permeability copper</t>
+  </si>
+  <si>
+    <t>Note: Green means I got the number from the paper, orange means I assumed it, red means there is a issue with the value in the paper.</t>
+  </si>
+  <si>
+    <t>Note: The assumptions I made I think can be explained. Conductivity of airgap was likely assumed to be 0, copper is not needed since it only occurs in the MEC region because sigma is only used in the lambda variable. All the permeabilities in other than iron were likely assumed to be 1.</t>
+  </si>
+  <si>
+    <t>One of the true inconsistencies is the MMF in the 2019 paper that didn’t exist in 2015 or 2018</t>
+  </si>
+  <si>
+    <t>Another great point about the MEC HM boundary is that I can always write a test script to check that my complex fourier series of the Bx_MEC is correct. I can do this by plotting the (Phi_xn + Phi_xp)/2urSyz for each K. Then plot the complex fourier series of this</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,8 +594,22 @@
       <charset val="161"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +662,22 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -543,7 +712,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -552,8 +721,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -596,14 +768,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="11">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
     <cellStyle name="20% - Accent5" xfId="5" builtinId="46"/>
     <cellStyle name="20% - Accent6" xfId="6" builtinId="50"/>
+    <cellStyle name="40% - Accent2" xfId="10" builtinId="35"/>
+    <cellStyle name="Accent2" xfId="9" builtinId="33"/>
     <cellStyle name="Bad" xfId="7" builtinId="27"/>
+    <cellStyle name="Good" xfId="8" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1862,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3280,16 +3467,19 @@
     </row>
     <row r="58" spans="1:9" ht="285" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>67</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>66</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3312,14 +3502,12 @@
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
     </row>
-    <row r="62" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
-        <v>111</v>
+    <row r="62" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
+        <v>160</v>
       </c>
       <c r="B62" s="7"/>
-      <c r="C62" s="15" t="s">
-        <v>112</v>
-      </c>
+      <c r="C62" s="15"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
@@ -3348,7 +3536,7 @@
   <dimension ref="A1:EB26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4550,4 +4738,321 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470EA571-87DB-4BDA-819A-DD9B46927D19}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="16"/>
+    <col min="5" max="5" width="31.5703125" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="17">
+        <v>3</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="17">
+        <v>6</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="17">
+        <v>16</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="17">
+        <v>57</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="17">
+        <v>50</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="19">
+        <v>12</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="17">
+        <v>6</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="17">
+        <v>10</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="17">
+        <v>20</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="17">
+        <v>6.5</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="17">
+        <v>2.7</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="17">
+        <v>2</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="17">
+        <v>8</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="17">
+        <v>1000</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="18">
+        <v>1</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="18">
+        <v>1</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="18">
+        <v>1</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Clean up the folder dirs and updates to the Complex Fourier Transform
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\MaSc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD292ED-09A1-4A8C-BD18-6BB131E921C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBDA2B8-7817-457B-8054-8569018F5F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="2" r:id="rId1"/>
@@ -541,7 +541,7 @@
     <t>One of the true inconsistencies is the MMF in the 2019 paper that didn’t exist in 2015 or 2018</t>
   </si>
   <si>
-    <t>Another great point about the MEC HM boundary is that I can always write a test script to check that my complex fourier series of the Bx_MEC is correct. I can do this by plotting the (Phi_xn + Phi_xp)/2urSyz for each K. Then plot the complex fourier series of this</t>
+    <t>Something interesting is that when plotting the Bx field in the boundary I see the max/min at 0.035/-0.035 which is roughly the same as the aigrap B field plot (too low) then that tells me the issue is elsewhere not in the boundary equation but in the B field plot since it happened when changing mesh density in this test too!</t>
   </si>
 </sst>
 </file>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3502,7 +3502,7 @@
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
     </row>
-    <row r="62" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
         <v>160</v>
       </c>

</xml_diff>

<commit_message>
Updates to Compute for plotting Bx at MEC-HM boundary
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB566F6-B504-4D03-834D-B04AD86E8783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8664E63B-D875-4930-BEAE-E3EAA3A0D2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="360" windowWidth="21600" windowHeight="11385" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="167">
   <si>
     <t>File</t>
   </si>
@@ -545,6 +545,21 @@
   </si>
   <si>
     <t>An interesting thought is that with a low mesh density the f value will be constant for a much longer node length lx compared to a dense mesh. Although both plots have an area equal to 0, the course mesh has more error but the next ones are not converging to a point. We should plot the difference between them to see if there is a convergence</t>
+  </si>
+  <si>
+    <t>If I find out that this is normal behaviour with the peaks of MMF dropping with finer mesh, then this tells me that the issue lies elsewhere and that I have to continue from the beginning</t>
+  </si>
+  <si>
+    <t>Worst case just send a message to the authors asking for more supplementary material. Send proof that Im actually far into solving it. Ask Solange for help</t>
+  </si>
+  <si>
+    <t>Try to upgrade my meshing to allow an input number of nodes in the x and y direction</t>
+  </si>
+  <si>
+    <t>Look into the Kc value for possibly being the entire coil span</t>
+  </si>
+  <si>
+    <t>What is weird is that the shape of each node makes a HUGE impact on the results. Look into if you need to keep the nodes in the x and y direction for a region the same? Ex) a coil needs to be square in terms of nodes in it</t>
   </si>
 </sst>
 </file>
@@ -2052,8 +2067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3512,13 +3527,26 @@
       <c r="B62" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="C62" s="15"/>
+      <c r="C62" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="7"/>
+    <row r="64" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+      <c r="A64" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>

</xml_diff>

<commit_message>
Important Ip must be initialized as np var
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C6B651-B849-438D-97E4-A95A116692B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E247D5-A693-4450-B391-784DA68983F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1365" windowWidth="27000" windowHeight="14235" activeTab="3" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
+    <workbookView xWindow="0" yWindow="1365" windowWidth="27000" windowHeight="14235" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="167">
   <si>
     <t>File</t>
   </si>
@@ -260,12 +260,6 @@
   </si>
   <si>
     <t>If there is a * in the comment it means I have checked the method for different len(n) values and different mecRegionLengths</t>
-  </si>
-  <si>
-    <t>Note: What is interesting from the note on the left is that as I increase pixelDiv, the error seen in the linalg_lu solution is still very low and stays roughly constant meaning that linalg_lu is valid for all but the values being passed in may be garbage</t>
-  </si>
-  <si>
-    <t>Try different values for pixelDiv and write down all the expected values on the excel sheet like Y_bc and the indexes</t>
   </si>
   <si>
     <t>ppAirBuffer</t>
@@ -398,9 +392,6 @@
     <t>One possible thing to try if all else fails is to transpose the coordinate system of tkinter to be normal in case that messed me up somewhere</t>
   </si>
   <si>
-    <t>Note: the airgap plot looks more correct at Div = 2 than Div = 15 which makes me think there is an error in the mec region</t>
-  </si>
-  <si>
     <t>Np</t>
   </si>
   <si>
@@ -539,30 +530,6 @@
     <t>Note: The assumptions I made I think can be explained. Conductivity of airgap was likely assumed to be 0, copper is not needed since it only occurs in the MEC region because sigma is only used in the lambda variable. All the permeabilities in other than iron were likely assumed to be 1.</t>
   </si>
   <si>
-    <t>One of the true inconsistencies is the MMF in the 2019 paper that didn’t exist in 2015 or 2018</t>
-  </si>
-  <si>
-    <t>Something interesting is that when plotting the Bx field in the boundary I see the max/min at 0.035/-0.035 which is roughly the same as the aigrap B field plot (too low) then that tells me the issue is elsewhere not in the boundary equation but in the B field plot since it happened when changing mesh density in this test too!</t>
-  </si>
-  <si>
-    <t>An interesting thought is that with a low mesh density the f value will be constant for a much longer node length lx compared to a dense mesh. Although both plots have an area equal to 0, the course mesh has more error but the next ones are not converging to a point. We should plot the difference between them to see if there is a convergence</t>
-  </si>
-  <si>
-    <t>If I find out that this is normal behaviour with the peaks of MMF dropping with finer mesh, then this tells me that the issue lies elsewhere and that I have to continue from the beginning</t>
-  </si>
-  <si>
-    <t>Worst case just send a message to the authors asking for more supplementary material. Send proof that Im actually far into solving it. Ask Solange for help</t>
-  </si>
-  <si>
-    <t>Try to upgrade my meshing to allow an input number of nodes in the x and y direction</t>
-  </si>
-  <si>
-    <t>Look into the Kc value for possibly being the entire coil span</t>
-  </si>
-  <si>
-    <t>What is weird is that the shape of each node makes a HUGE impact on the results. Look into if you need to keep the nodes in the x and y direction for a region the same? Ex) a coil needs to be square in terms of nodes in it</t>
-  </si>
-  <si>
     <t>PixelDivs</t>
   </si>
   <si>
@@ -591,6 +558,9 @@
   </si>
   <si>
     <t>ppSlotheight//2</t>
+  </si>
+  <si>
+    <t>I can try to plot the results for different meshes again to see what the outcome is and how consistent the meshing and B field is</t>
   </si>
 </sst>
 </file>
@@ -9921,8 +9891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10315,7 +10285,7 @@
         <v>100</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F16" s="7" t="str">
         <v>LIM_Compute</v>
@@ -10389,7 +10359,7 @@
         <v>100</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F19" s="7" t="str">
         <v>LIM_Compute</v>
@@ -10679,7 +10649,7 @@
         <v>100</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F31" s="7" t="str">
         <v>LIM_Compute</v>
@@ -11337,70 +11307,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="285" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>67</v>
+        <v>106</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>107</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E58" s="15" t="s">
-        <v>159</v>
-      </c>
+      <c r="E58" s="15"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
     </row>
-    <row r="60" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>108</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>110</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
     </row>
-    <row r="62" spans="1:9" ht="285" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>163</v>
-      </c>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="15"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="1:9" ht="255" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>166</v>
-      </c>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="15"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>
@@ -11434,7 +11381,7 @@
   <sheetData>
     <row r="1" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1" s="9">
         <v>12</v>
@@ -11442,13 +11389,13 @@
     </row>
     <row r="2" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="8">
         <v>116</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -11473,13 +11420,13 @@
     </row>
     <row r="3" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" s="8">
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
@@ -11510,7 +11457,7 @@
     </row>
     <row r="4" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="8">
         <v>6</v>
@@ -11581,14 +11528,14 @@
     </row>
     <row r="5" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" s="8">
         <v>1</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F5" s="8">
         <v>3</v>
@@ -11620,14 +11567,14 @@
     </row>
     <row r="6" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" s="8">
         <v>35</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F6" s="8">
         <v>7</v>
@@ -11667,14 +11614,14 @@
     </row>
     <row r="7" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" s="8">
         <v>20</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F7" s="8">
         <v>15</v>
@@ -11714,13 +11661,13 @@
     </row>
     <row r="8" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="8">
         <v>432</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E8" s="8">
         <v>23</v>
@@ -11749,13 +11696,13 @@
     </row>
     <row r="9" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" s="8">
         <v>6</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E9" s="8">
         <v>25</v>
@@ -11782,13 +11729,13 @@
     </row>
     <row r="10" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" s="8">
         <v>432</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E10" s="8">
         <v>26</v>
@@ -11825,13 +11772,13 @@
     </row>
     <row r="11" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11" s="8">
         <v>6</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E11" s="8">
         <v>32</v>
@@ -11862,7 +11809,7 @@
     </row>
     <row r="12" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12" s="8">
         <v>8</v>
@@ -11870,13 +11817,13 @@
     </row>
     <row r="13" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B13" s="8">
         <v>16</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E13" s="8">
         <v>122</v>
@@ -12265,13 +12212,13 @@
     </row>
     <row r="14" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B14" s="8">
         <v>12</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E14" s="8">
         <v>116</v>
@@ -12548,7 +12495,7 @@
     </row>
     <row r="15" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" s="8">
         <v>4</v>
@@ -12556,7 +12503,7 @@
     </row>
     <row r="16" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" s="8">
         <v>3</v>
@@ -12564,7 +12511,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B17" s="8">
         <v>3</v>
@@ -12572,7 +12519,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B18" s="8">
         <v>4</v>
@@ -12580,7 +12527,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B19" s="8">
         <v>16</v>
@@ -12588,7 +12535,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20" s="8">
         <v>8640</v>
@@ -12596,7 +12543,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B21" s="8">
         <v>100</v>
@@ -12604,22 +12551,22 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -12645,298 +12592,298 @@
   <sheetData>
     <row r="1" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C1" s="17">
         <v>3</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C2" s="17">
         <v>6</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C3" s="17">
         <v>16</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C4" s="17">
         <v>57</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C5" s="17">
         <v>50</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C6" s="19">
         <v>12</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C7" s="17">
         <v>6</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C8" s="17">
         <v>10</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C9" s="17">
         <v>20</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C10" s="17">
         <v>6.5</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C11" s="17">
         <v>2.7</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C12" s="17">
         <v>2</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C13" s="17">
         <v>8</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C18" s="17">
         <v>1000</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C19" s="18">
         <v>1</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C20" s="18">
         <v>1</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C21" s="18">
         <v>1</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -12948,7 +12895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE7A0CB-1887-4F0F-8F3A-7013480AD86F}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
@@ -12978,43 +12925,43 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
       <c r="J1" s="21" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E2" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="G2" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="H2" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="I2" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="J2" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="K2" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes to match 2019 pages
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E247D5-A693-4450-B391-784DA68983F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0DFE47-3062-4710-827D-730C0378CC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1365" windowWidth="27000" windowHeight="14235" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="179">
   <si>
     <t>File</t>
   </si>
@@ -561,13 +561,49 @@
   </si>
   <si>
     <t>I can try to plot the results for different meshes again to see what the outcome is and how consistent the meshing and B field is</t>
+  </si>
+  <si>
+    <t>Important to know that when running the comparison of the Bx value at each node a very small amount of error was seen in pixelDiv = 10 and up meaning You should run at this for efficient computing</t>
+  </si>
+  <si>
+    <t>To validate my meshing I can mesh the coils into a local square mesh or a rectangle mesh. Then validate my new scaling method is correct visually</t>
+  </si>
+  <si>
+    <t>DO IT NOW: I NEED TO EMAIL DR KAR ABOUT THE ANSYS HELP, THE FASTER THE BETTER (DON’T BE A PUSSY)</t>
+  </si>
+  <si>
+    <t>This proves that the meshing is working well since the MMF and Reluctance in the top row flexes with changes to ppSlotheight:2ppSlot ratio. When you look at the first column of graphs you see B field barely changes to the flex so MMF and R counter</t>
+  </si>
+  <si>
+    <t>Primary Length</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Look at the picture for compareAirgap in the Troubleshooting folder</t>
+  </si>
+  <si>
+    <t>Complex Fourier Series does not change the magnitude. Of the input waveform. This means that the MMF waveform determines everything about the final waveform in the middle of the airgap. This includes MMF and crossover points</t>
+  </si>
+  <si>
+    <t>What if I need to account for mmf in the y direction as well in the flux equations, unlikely but worth a try</t>
+  </si>
+  <si>
+    <t>Plot the By plot at the Boundary</t>
+  </si>
+  <si>
+    <t>Check the Vect Pot around the upper 2 left coils</t>
+  </si>
+  <si>
+    <t>Why am I getting linalg error at pixelDiv = 5. This is a serious issue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,8 +663,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -691,12 +742,6 @@
         <fgColor theme="5"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -731,7 +776,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -742,9 +787,8 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -793,26 +837,31 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
     <cellStyle name="20% - Accent5" xfId="5" builtinId="46"/>
     <cellStyle name="20% - Accent6" xfId="6" builtinId="50"/>
-    <cellStyle name="40% - Accent2" xfId="10" builtinId="35"/>
     <cellStyle name="Accent2" xfId="9" builtinId="33"/>
     <cellStyle name="Bad" xfId="7" builtinId="27"/>
     <cellStyle name="Good" xfId="8" builtinId="26"/>
@@ -1247,7 +1296,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$I$2</c:f>
+              <c:f>PlotCorrelation!$I$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1281,57 +1330,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$I$3:$I$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$I$4:$I$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$I$5:$I$8</c:f>
+              <c:f>PlotCorrelation!$I$4:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>79.167000000000002</c:v>
+                  <c:v>249.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59.375</c:v>
+                  <c:v>256.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.344000000000001</c:v>
+                  <c:v>223.93</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.875</c:v>
+                  <c:v>267.1875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1364,7 +1412,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$B$2</c:f>
+              <c:f>PlotCorrelation!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1398,57 +1446,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$B$3:$B$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$B$4:$B$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$B$5:$B$8</c:f>
+              <c:f>PlotCorrelation!$B$4:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1491,57 +1538,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$D$3:$D$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$D$4:$D$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$D$5:$D$8</c:f>
+              <c:f>PlotCorrelation!$D$4:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1901,7 +1947,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$I$2</c:f>
+              <c:f>PlotCorrelation!$I$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1935,57 +1981,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$I$3:$I$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$I$4:$I$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$I$5:$I$8</c:f>
+              <c:f>PlotCorrelation!$I$4:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>79.167000000000002</c:v>
+                  <c:v>249.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59.375</c:v>
+                  <c:v>256.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.344000000000001</c:v>
+                  <c:v>223.93</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.875</c:v>
+                  <c:v>267.1875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2018,7 +2063,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$E$2</c:f>
+              <c:f>PlotCorrelation!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2052,57 +2097,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$E$3:$E$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$E$4:$E$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$E$5:$E$8</c:f>
+              <c:f>PlotCorrelation!$E$4:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.3E-3</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.4E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.25E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2145,57 +2189,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$F$3:$F$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$F$4:$F$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$F$5:$F$8</c:f>
+              <c:f>PlotCorrelation!$F$4:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.3E-3</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.6999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.25E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2551,7 +2594,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$G$2</c:f>
+              <c:f>PlotCorrelation!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2585,43 +2628,42 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$G$3:$G$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$G$4:$G$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$G$5:$G$8</c:f>
+              <c:f>PlotCorrelation!$G$4:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2629,13 +2671,13 @@
                   <c:v>7957747.1545947604</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5968310.3659460703</c:v>
+                  <c:v>7957747.1545947604</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>6820926.1325097997</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>7957747.1545947604</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6366197.7236758098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2652,7 +2694,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$H$2</c:f>
+              <c:f>PlotCorrelation!$H$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2686,43 +2728,42 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$H$3:$H$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$H$4:$H$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$H$5:$H$8</c:f>
+              <c:f>PlotCorrelation!$H$4:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2730,13 +2771,13 @@
                   <c:v>7957747.1545947604</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10610329.539459599</c:v>
+                  <c:v>7957747.1545947604</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>9284038.3470272198</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>7957747.1545947604</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9947183.9432434496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2769,7 +2810,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$B$2</c:f>
+              <c:f>PlotCorrelation!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2803,57 +2844,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$B$3:$B$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$B$4:$B$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$B$5:$B$8</c:f>
+              <c:f>PlotCorrelation!$B$4:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2870,7 +2910,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$D$2</c:f>
+              <c:f>PlotCorrelation!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2904,57 +2944,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$D$3:$D$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$D$4:$D$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$D$5:$D$8</c:f>
+              <c:f>PlotCorrelation!$D$4:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3310,7 +3349,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$G$2</c:f>
+              <c:f>PlotCorrelation!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3344,43 +3383,42 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$G$3:$G$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$G$4:$G$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$G$5:$G$8</c:f>
+              <c:f>PlotCorrelation!$G$4:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3388,13 +3426,13 @@
                   <c:v>7957747.1545947604</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5968310.3659460703</c:v>
+                  <c:v>7957747.1545947604</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>6820926.1325097997</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>7957747.1545947604</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6366197.7236758098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3411,7 +3449,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$H$2</c:f>
+              <c:f>PlotCorrelation!$H$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3445,43 +3483,42 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$H$3:$H$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$H$4:$H$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$H$5:$H$8</c:f>
+              <c:f>PlotCorrelation!$H$4:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3489,13 +3526,13 @@
                   <c:v>7957747.1545947604</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10610329.539459599</c:v>
+                  <c:v>7957747.1545947604</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>9284038.3470272198</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>7957747.1545947604</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9947183.9432434496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3528,7 +3565,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$E$2</c:f>
+              <c:f>PlotCorrelation!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3562,57 +3599,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$E$3:$E$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$E$4:$E$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$E$5:$E$8</c:f>
+              <c:f>PlotCorrelation!$E$4:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.3E-3</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.4E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.25E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3655,57 +3691,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$F$3:$F$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$F$4:$F$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$F$5:$F$8</c:f>
+              <c:f>PlotCorrelation!$F$4:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.3E-3</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.6999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.25E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4061,7 +4096,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$J$2</c:f>
+              <c:f>PlotCorrelation!$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4095,57 +4130,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$J$3:$J$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$J$4:$J$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$J$5:$J$8</c:f>
+              <c:f>PlotCorrelation!$J$4:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.01</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.01</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0000000000000002E-3</c:v>
+                  <c:v>3.0200000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0000000000000002E-3</c:v>
+                  <c:v>3.0099999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4162,7 +4196,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$K$2</c:f>
+              <c:f>PlotCorrelation!$K$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4196,57 +4230,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$K$3:$K$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$K$4:$K$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$K$5:$K$8</c:f>
+              <c:f>PlotCorrelation!$K$4:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>-3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>-3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>-3.0499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>-3.0700000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4279,7 +4312,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$B$2</c:f>
+              <c:f>PlotCorrelation!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4313,57 +4346,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$B$3:$B$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$B$4:$B$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$B$5:$B$8</c:f>
+              <c:f>PlotCorrelation!$B$4:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4380,7 +4412,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$D$2</c:f>
+              <c:f>PlotCorrelation!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4414,57 +4446,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$D$3:$D$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$D$4:$D$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$D$5:$D$8</c:f>
+              <c:f>PlotCorrelation!$D$4:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4820,7 +4851,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$J$2</c:f>
+              <c:f>PlotCorrelation!$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4854,57 +4885,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$J$3:$J$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$J$4:$J$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$J$5:$J$8</c:f>
+              <c:f>PlotCorrelation!$J$4:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.01</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.01</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0000000000000002E-3</c:v>
+                  <c:v>3.0200000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0000000000000002E-3</c:v>
+                  <c:v>3.0099999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4921,7 +4951,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$K$2</c:f>
+              <c:f>PlotCorrelation!$K$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4955,57 +4985,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$K$3:$K$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$K$4:$K$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$K$5:$K$8</c:f>
+              <c:f>PlotCorrelation!$K$4:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>-3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>-3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>-3.0499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>-3.0700000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5038,7 +5067,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>PlotCorrelation!$E$2</c:f>
+              <c:f>PlotCorrelation!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5072,57 +5101,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$E$3:$E$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$E$4:$E$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$E$5:$E$8</c:f>
+              <c:f>PlotCorrelation!$E$4:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.3E-3</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.4E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.25E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5165,57 +5193,56 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$A$3:$A$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$A$4:$A$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:f>PlotCorrelation!$A$4:$A$7</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PlotCorrelation!$F$3:$F$8</c15:sqref>
+                    <c15:sqref>PlotCorrelation!$F$4:$F$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>PlotCorrelation!$F$5:$F$8</c:f>
+              <c:f>PlotCorrelation!$F$4:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.3E-3</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.6999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.25E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9354,13 +9381,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9390,13 +9417,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9428,13 +9455,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9466,13 +9493,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9504,13 +9531,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9542,13 +9569,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9891,8 +9918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10381,7 +10408,7 @@
       <c r="B20" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="23">
         <v>100</v>
       </c>
       <c r="D20" s="3"/>
@@ -11325,29 +11352,47 @@
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
     </row>
-    <row r="60" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>108</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>166</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
+    <row r="62" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="15"/>
+    <row r="64" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A64" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>
@@ -12576,10 +12621,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470EA571-87DB-4BDA-819A-DD9B46927D19}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12667,16 +12712,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="18">
         <v>12</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>116</v>
       </c>
     </row>
@@ -12807,26 +12852,26 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="17" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="17" t="s">
         <v>130</v>
       </c>
     </row>
@@ -12845,45 +12890,56 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="17">
         <v>1</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="17" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="17">
         <v>1</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="17" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="17">
         <v>1</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="17" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C22" s="16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -12893,10 +12949,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE7A0CB-1887-4F0F-8F3A-7013480AD86F}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12904,121 +12960,103 @@
     <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>50</v>
+        <v>168</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21" t="s">
-        <v>14</v>
-      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
-      <c r="J1" s="21" t="s">
-        <v>162</v>
-      </c>
+      <c r="J1" s="21"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" s="21"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>156</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>77</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>78</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>165</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>157</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>158</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
         <v>160</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H3" t="s">
         <v>161</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I3" t="s">
         <v>159</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J3" t="s">
         <v>163</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <f>C3/2</f>
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0.01</v>
-      </c>
-      <c r="F3">
-        <v>0.01</v>
-      </c>
-      <c r="G3">
-        <v>7957747.1545947604</v>
-      </c>
-      <c r="H3">
-        <v>7957747.1545947604</v>
-      </c>
-      <c r="I3">
-        <v>142.5</v>
-      </c>
-      <c r="J3">
-        <v>0.03</v>
-      </c>
-      <c r="K3">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <f>C4/2</f>
         <v>4</v>
       </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D8" si="0">C4/2</f>
-        <v>2</v>
-      </c>
       <c r="E4">
-        <v>5.0000000000000001E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="F4">
-        <v>5.0000000000000001E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="G4">
         <v>7957747.1545947604</v>
@@ -13027,34 +13065,34 @@
         <v>7957747.1545947604</v>
       </c>
       <c r="I4">
-        <v>106.875</v>
+        <v>249.375</v>
       </c>
       <c r="J4">
-        <v>1.4999999999999999E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K4">
-        <v>0.02</v>
+        <v>-3.1E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" ref="D5:D7" si="0">C5/2</f>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>3.3E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="F5">
-        <v>3.3E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="G5">
         <v>7957747.1545947604</v>
@@ -13063,70 +13101,70 @@
         <v>7957747.1545947604</v>
       </c>
       <c r="I5">
-        <v>79.167000000000002</v>
+        <v>256.5</v>
       </c>
       <c r="J5">
-        <v>0.01</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K5">
-        <v>1.4999999999999999E-2</v>
+        <v>-3.1E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>2.5000000000000001E-3</v>
+        <v>1.4E-3</v>
       </c>
       <c r="F6">
-        <v>3.3E-3</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="G6">
-        <v>5968310.3659460703</v>
+        <v>6820926.1325097997</v>
       </c>
       <c r="H6">
-        <v>10610329.539459599</v>
+        <v>9284038.3470272198</v>
       </c>
       <c r="I6">
-        <v>59.375</v>
+        <v>223.93</v>
       </c>
       <c r="J6">
-        <v>0.01</v>
+        <v>3.0200000000000001E-2</v>
       </c>
       <c r="K6">
-        <v>1.4999999999999999E-2</v>
+        <v>-3.0499999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>2.5000000000000001E-3</v>
+        <v>1.25E-3</v>
       </c>
       <c r="F7">
-        <v>2.5000000000000001E-3</v>
+        <v>1.25E-3</v>
       </c>
       <c r="G7">
         <v>7957747.1545947604</v>
@@ -13135,56 +13173,47 @@
         <v>7957747.1545947604</v>
       </c>
       <c r="I7">
-        <v>62.344000000000001</v>
+        <v>267.1875</v>
       </c>
       <c r="J7">
-        <v>8.0000000000000002E-3</v>
+        <v>3.0099999999999998E-2</v>
       </c>
       <c r="K7">
-        <v>1.4999999999999999E-2</v>
+        <v>-3.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <v>2E-3</v>
-      </c>
-      <c r="F8">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="G8">
-        <v>6366197.7236758098</v>
-      </c>
-      <c r="H8">
-        <v>9947183.9432434496</v>
-      </c>
-      <c r="I8">
-        <v>49.875</v>
-      </c>
-      <c r="J8">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="K8">
-        <v>1.4999999999999999E-2</v>
-      </c>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="A1:C1"/>
+  <mergeCells count="5">
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A9:U9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updates to Show.py to understand the visualization of matrix B and colour grading improvements
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0DFE47-3062-4710-827D-730C0378CC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC11BBF-A10D-4E45-99D7-5D899B6C92F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="183">
   <si>
     <t>File</t>
   </si>
@@ -596,7 +596,19 @@
     <t>Check the Vect Pot around the upper 2 left coils</t>
   </si>
   <si>
-    <t>Why am I getting linalg error at pixelDiv = 5. This is a serious issue</t>
+    <t>3) Look into other equations (hmMec)</t>
+  </si>
+  <si>
+    <t>2) Look at scalar potential after solving linalg near the coils and see where it tapers off using Show</t>
+  </si>
+  <si>
+    <t>4) Try to visualize the By BC between MEC and HM</t>
+  </si>
+  <si>
+    <t>I feel like there is contribution from the upper coil in the waveform but this contribution is minor compared to the right side lower coils. This could be due to the boundary condition Bx</t>
+  </si>
+  <si>
+    <t>Visually draw on the Bx matplots markers where the upper and lower coils start</t>
   </si>
 </sst>
 </file>
@@ -846,14 +858,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -9916,10 +9928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10408,7 +10420,7 @@
       <c r="B20" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="21">
         <v>100</v>
       </c>
       <c r="D20" s="3"/>
@@ -11376,9 +11388,7 @@
       <c r="B62" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="C62" s="15" t="s">
-        <v>178</v>
-      </c>
+      <c r="C62" s="15"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
@@ -11394,11 +11404,29 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="7"/>
+    <row r="66" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B66" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A69" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>182</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12970,38 +12998,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="K2" s="21"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -13183,29 +13211,29 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
-      <c r="U9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Update Wireframe in Show, include all MMF sources in mecHm BC in Compute, update pixels in Grid
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC11BBF-A10D-4E45-99D7-5D899B6C92F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F2BE5E-E663-459C-8C96-E00D06AA007F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
+    <workbookView xWindow="1155" yWindow="0" windowWidth="14730" windowHeight="15600" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="183">
   <si>
     <t>File</t>
   </si>
@@ -371,9 +371,6 @@
   </si>
   <si>
     <t>Assuming my math is right</t>
-  </si>
-  <si>
-    <t>TODO for 2/Tper but I calculated 1/Tper. I still need to review my math with someone for the understanding of this boundary condition</t>
   </si>
   <si>
     <t>The worst case error is e^-17 and propogates to roughly e^-14 when calculating B field. This is still negligible</t>
@@ -581,9 +578,6 @@
     <t>m</t>
   </si>
   <si>
-    <t>Look at the picture for compareAirgap in the Troubleshooting folder</t>
-  </si>
-  <si>
     <t>Complex Fourier Series does not change the magnitude. Of the input waveform. This means that the MMF waveform determines everything about the final waveform in the middle of the airgap. This includes MMF and crossover points</t>
   </si>
   <si>
@@ -605,10 +599,23 @@
     <t>4) Try to visualize the By BC between MEC and HM</t>
   </si>
   <si>
-    <t>I feel like there is contribution from the upper coil in the waveform but this contribution is minor compared to the right side lower coils. This could be due to the boundary condition Bx</t>
-  </si>
-  <si>
     <t>Visually draw on the Bx matplots markers where the upper and lower coils start</t>
+  </si>
+  <si>
+    <t>1) The error could also be in the post-processing math as well</t>
+  </si>
+  <si>
+    <t>When increasing the MMF of only the top layer windings, I see no change in the result but when I do this for the lower level there is a change</t>
+  </si>
+  <si>
+    <t>I am confident the post processing code is correct after linalg
+The interesting thing is my magnitude is roughly correct now but the waveform is still really wrong
+Compared to the 2019 results, it looks almost like my waveform is mirrored in the x axis
+- This could be due to bad phase rotation or bad boundary conditions
+Today I checked and upgraded the mecHm equations to include all the MMF (this may still be wrong)
+I checked the MEC region equations last and was happy with that (cannot trust 100% though)
+What are the next steps?
+Plot Yk and check the vals for the left coils. Try this with different MMF cancelling</t>
   </si>
 </sst>
 </file>
@@ -1092,10 +1099,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5500</c:v>
+                  <c:v>5300</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1107,10 +1114,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5500</c:v>
+                  <c:v>5300</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9928,10 +9935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9987,13 +9994,13 @@
       <c r="D2" s="2"/>
       <c r="F2" s="7" t="str" cm="1">
         <f t="array" ref="F2:I56">_xlfn._xlws.SORT(TrackIssues5[], 3, 1)</f>
-        <v>LIM_SlotPoleCalculation</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G2" s="7" t="str">
-        <v>LimMotor</v>
+        <v>finalizeCompute</v>
       </c>
       <c r="H2" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I2" s="7">
         <v>0</v>
@@ -10011,13 +10018,13 @@
       </c>
       <c r="D3" s="2"/>
       <c r="F3" s="7" t="str">
-        <v>LIM_SlotPoleCalculation</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G3" s="7" t="str">
-        <v>Error</v>
+        <v>updateGrid</v>
       </c>
       <c r="H3" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I3" s="7">
         <v>0</v>
@@ -10038,7 +10045,7 @@
         <v>LIM_SlotPoleCalculation</v>
       </c>
       <c r="G4" s="7" t="str">
-        <v>np_find_nearest</v>
+        <v>LimMotor</v>
       </c>
       <c r="H4" s="7">
         <v>100</v>
@@ -10062,7 +10069,7 @@
         <v>LIM_SlotPoleCalculation</v>
       </c>
       <c r="G5" s="7" t="str">
-        <v>timing</v>
+        <v>Error</v>
       </c>
       <c r="H5" s="7">
         <v>100</v>
@@ -10085,16 +10092,16 @@
         <v>49</v>
       </c>
       <c r="F6" s="7" t="str">
-        <v>LIM_Grid</v>
+        <v>LIM_SlotPoleCalculation</v>
       </c>
       <c r="G6" s="7" t="str">
-        <v>Grid</v>
+        <v>np_find_nearest</v>
       </c>
       <c r="H6" s="7">
         <v>100</v>
       </c>
-      <c r="I6" s="7" t="str">
-        <v>small source for error is sigma is not exact and rather is 1 or 0 which can be improved. I think we should comb through Grid class to make sure its mostly np.array not lists and clean it up</v>
+      <c r="I6" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -10109,10 +10116,10 @@
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="7" t="str">
-        <v>LIM_Grid</v>
+        <v>LIM_SlotPoleCalculation</v>
       </c>
       <c r="G7" s="7" t="str">
-        <v>Node</v>
+        <v>timing</v>
       </c>
       <c r="H7" s="7">
         <v>100</v>
@@ -10136,13 +10143,13 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G8" s="7" t="str">
-        <v>Region</v>
+        <v>Grid</v>
       </c>
       <c r="H8" s="7">
         <v>100</v>
       </c>
-      <c r="I8" s="7">
-        <v>0</v>
+      <c r="I8" s="7" t="str">
+        <v>small source for error is sigma is not exact and rather is 1 or 0 which can be improved. I think we should comb through Grid class to make sure its mostly np.array not lists and clean it up</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -10160,7 +10167,7 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G9" s="7" t="str">
-        <v>reluctance</v>
+        <v>Node</v>
       </c>
       <c r="H9" s="7">
         <v>100</v>
@@ -10184,7 +10191,7 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G10" s="7" t="str">
-        <v>meshBoundary</v>
+        <v>Region</v>
       </c>
       <c r="H10" s="7">
         <v>100</v>
@@ -10208,7 +10215,7 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G11" s="7" t="str">
-        <v>checkSpatialMapping</v>
+        <v>reluctance</v>
       </c>
       <c r="H11" s="7">
         <v>100</v>
@@ -10232,7 +10239,7 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G12" s="7" t="str">
-        <v>buildGrid</v>
+        <v>meshBoundary</v>
       </c>
       <c r="H12" s="7">
         <v>100</v>
@@ -10256,7 +10263,7 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G13" s="7" t="str">
-        <v>setRegionIndices</v>
+        <v>checkSpatialMapping</v>
       </c>
       <c r="H13" s="7">
         <v>100</v>
@@ -10280,7 +10287,7 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G14" s="7" t="str">
-        <v>finalizeGrid</v>
+        <v>buildGrid</v>
       </c>
       <c r="H14" s="7">
         <v>100</v>
@@ -10301,10 +10308,10 @@
       </c>
       <c r="D15" s="3"/>
       <c r="F15" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_Grid</v>
       </c>
       <c r="G15" s="7" t="str">
-        <v>Model</v>
+        <v>setRegionIndices</v>
       </c>
       <c r="H15" s="7">
         <v>100</v>
@@ -10324,19 +10331,19 @@
         <v>100</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F16" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_Grid</v>
       </c>
       <c r="G16" s="7" t="str">
-        <v>linalg_lu</v>
+        <v>finalizeGrid</v>
       </c>
       <c r="H16" s="7">
         <v>100</v>
       </c>
-      <c r="I16" s="7" t="str">
-        <v>The worst case error is e^-17 and propogates to roughly e^-14 when calculating B field. This is still negligible</v>
+      <c r="I16" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -10354,7 +10361,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G17" s="7" t="str">
-        <v>dirichlet</v>
+        <v>Model</v>
       </c>
       <c r="H17" s="7">
         <v>100</v>
@@ -10378,23 +10385,23 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G18" s="7" t="str">
-        <v>hmHm</v>
+        <v>linalg_lu</v>
       </c>
       <c r="H18" s="7">
         <v>100</v>
       </c>
-      <c r="I18" s="7">
-        <v>0</v>
+      <c r="I18" s="7" t="str">
+        <v>The worst case error is e^-17 and propogates to roughly e^-14 when calculating B field. This is still negligible</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="21">
         <v>100</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -10404,13 +10411,13 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G19" s="7" t="str">
-        <v>mecHm</v>
+        <v>dirichlet</v>
       </c>
       <c r="H19" s="7">
         <v>100</v>
       </c>
-      <c r="I19" s="7" t="str">
-        <v>TODO for 2/Tper but I calculated 1/Tper. I still need to review my math with someone for the understanding of this boundary condition</v>
+      <c r="I19" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -10428,7 +10435,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G20" s="7" t="str">
-        <v>mec</v>
+        <v>hmHm</v>
       </c>
       <c r="H20" s="7">
         <v>100</v>
@@ -10452,13 +10459,13 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G21" s="7" t="str">
-        <v>preEqn24_2018</v>
+        <v>mecHm</v>
       </c>
       <c r="H21" s="7">
         <v>100</v>
       </c>
-      <c r="I21" s="7">
-        <v>0</v>
+      <c r="I21" s="7" t="str">
+        <v>The worst case error is e^-17 and propogates to roughly e^-14 when calculating B field. This is still negligible</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -10476,7 +10483,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G22" s="7" t="str">
-        <v>preEqn25_2018</v>
+        <v>mec</v>
       </c>
       <c r="H22" s="7">
         <v>100</v>
@@ -10500,7 +10507,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G23" s="7" t="str">
-        <v>postMECAvgB</v>
+        <v>preEqn24_2018</v>
       </c>
       <c r="H23" s="7">
         <v>100</v>
@@ -10524,7 +10531,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G24" s="7" t="str">
-        <v>preEqn8</v>
+        <v>preEqn25_2018</v>
       </c>
       <c r="H24" s="7">
         <v>100</v>
@@ -10548,7 +10555,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G25" s="7" t="str">
-        <v>postEqn8</v>
+        <v>postMECAvgB</v>
       </c>
       <c r="H25" s="7">
         <v>100</v>
@@ -10572,7 +10579,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G26" s="7" t="str">
-        <v>postEqn9</v>
+        <v>preEqn8</v>
       </c>
       <c r="H26" s="7">
         <v>100</v>
@@ -10596,7 +10603,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G27" s="7" t="str">
-        <v>postEqn14to15</v>
+        <v>postEqn8</v>
       </c>
       <c r="H27" s="7">
         <v>100</v>
@@ -10620,7 +10627,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G28" s="7" t="str">
-        <v>postEqn16to17</v>
+        <v>postEqn9</v>
       </c>
       <c r="H28" s="7">
         <v>100</v>
@@ -10644,7 +10651,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G29" s="7" t="str">
-        <v>preEqn21</v>
+        <v>postEqn14to15</v>
       </c>
       <c r="H29" s="7">
         <v>100</v>
@@ -10668,7 +10675,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G30" s="7" t="str">
-        <v>postEqn21</v>
+        <v>postEqn16to17</v>
       </c>
       <c r="H30" s="7">
         <v>100</v>
@@ -10694,13 +10701,13 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G31" s="7" t="str">
-        <v>eqn23Integral</v>
+        <v>preEqn21</v>
       </c>
       <c r="H31" s="7">
         <v>100</v>
       </c>
-      <c r="I31" s="7" t="str">
-        <v>Assuming my math is right</v>
+      <c r="I31" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -10718,7 +10725,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G32" s="7" t="str">
-        <v>checkForErrors</v>
+        <v>postEqn21</v>
       </c>
       <c r="H32" s="7">
         <v>100</v>
@@ -10742,13 +10749,13 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G33" s="7" t="str">
-        <v>neighbourNodes</v>
+        <v>eqn23Integral</v>
       </c>
       <c r="H33" s="7">
         <v>100</v>
       </c>
-      <c r="I33" s="7">
-        <v>0</v>
+      <c r="I33" s="7" t="str">
+        <v>Assuming my math is right</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -10766,7 +10773,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G34" s="7" t="str">
-        <v>boundaryInfo</v>
+        <v>checkForErrors</v>
       </c>
       <c r="H34" s="7">
         <v>100</v>
@@ -10790,7 +10797,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G35" s="7" t="str">
-        <v>reduceMatrix</v>
+        <v>neighbourNodes</v>
       </c>
       <c r="H35" s="7">
         <v>100</v>
@@ -10814,7 +10821,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G36" s="7" t="str">
-        <v>buildMatAB</v>
+        <v>boundaryInfo</v>
       </c>
       <c r="H36" s="7">
         <v>100</v>
@@ -10838,7 +10845,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G37" s="7" t="str">
-        <v>updateLists</v>
+        <v>reduceMatrix</v>
       </c>
       <c r="H37" s="7">
         <v>100</v>
@@ -10862,7 +10869,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G38" s="7" t="str">
-        <v>shiftHmIdxList</v>
+        <v>buildMatAB</v>
       </c>
       <c r="H38" s="7">
         <v>100</v>
@@ -10879,14 +10886,14 @@
         <v>54</v>
       </c>
       <c r="C39" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D39" s="3"/>
       <c r="F39" s="7" t="str">
         <v>LIM_Compute</v>
       </c>
       <c r="G39" s="7" t="str">
-        <v>finalizeCompute</v>
+        <v>updateLists</v>
       </c>
       <c r="H39" s="7">
         <v>100</v>
@@ -10912,13 +10919,13 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G40" s="7" t="str">
-        <v>genForces</v>
+        <v>shiftHmIdxList</v>
       </c>
       <c r="H40" s="7">
         <v>100</v>
       </c>
-      <c r="I40" s="7" t="str">
-        <v>*</v>
+      <c r="I40" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -10936,13 +10943,13 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G41" s="7" t="str">
-        <v>plotPointsAlongX</v>
+        <v>genForces</v>
       </c>
       <c r="H41" s="7">
         <v>100</v>
       </c>
-      <c r="I41" s="7">
-        <v>0</v>
+      <c r="I41" s="7" t="str">
+        <v>*</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -10953,14 +10960,14 @@
         <v>52</v>
       </c>
       <c r="C42" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D42" s="3"/>
       <c r="F42" s="7" t="str">
         <v>LIM_Compute</v>
       </c>
       <c r="G42" s="7" t="str">
-        <v>updateGrid</v>
+        <v>plotPointsAlongX</v>
       </c>
       <c r="H42" s="7">
         <v>100</v>
@@ -11339,22 +11346,22 @@
       </c>
       <c r="C57" s="7">
         <f>SUM(TrackIssues5[Confidence])</f>
-        <v>5500</v>
+        <v>5300</v>
       </c>
       <c r="D57" s="7">
         <f>ROWS(TrackIssues5[Confidence]) *100 - C57</f>
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B58" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" s="15" t="s">
         <v>106</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>107</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>66</v>
@@ -11366,27 +11373,24 @@
     </row>
     <row r="60" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B60" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C60" s="7" t="s">
-        <v>167</v>
-      </c>
       <c r="D60" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
     </row>
-    <row r="62" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C62" s="15"/>
     </row>
@@ -11395,36 +11399,44 @@
     </row>
     <row r="64" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>
     </row>
     <row r="66" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>180</v>
+      </c>
       <c r="B66" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
         <v>181</v>
       </c>
       <c r="B69" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
         <v>182</v>
       </c>
     </row>
@@ -12665,306 +12677,306 @@
   <sheetData>
     <row r="1" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" s="17">
         <v>3</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="17">
         <v>6</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="17">
         <v>16</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="17">
         <v>57</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="17">
         <v>50</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="18">
         <v>12</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="17">
         <v>6</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" s="17">
         <v>10</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" s="17">
         <v>20</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" s="17">
         <v>6.5</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" s="17">
         <v>2.7</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" s="17">
         <v>2</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C13" s="17">
         <v>8</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C14" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>129</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" s="17">
         <v>1000</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19" s="17">
         <v>1</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C20" s="17">
         <v>1</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C21" s="17">
         <v>1</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>171</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>172</v>
       </c>
       <c r="C22" s="16">
         <v>0</v>
@@ -12999,7 +13011,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -13027,13 +13039,13 @@
       <c r="H2" s="22"/>
       <c r="I2" s="22"/>
       <c r="J2" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
@@ -13042,28 +13054,28 @@
         <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" t="s">
         <v>157</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H3" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" t="s">
         <v>158</v>
       </c>
-      <c r="G3" t="s">
-        <v>160</v>
-      </c>
-      <c r="H3" t="s">
-        <v>161</v>
-      </c>
-      <c r="I3" t="s">
-        <v>159</v>
-      </c>
       <c r="J3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K3" t="s">
         <v>163</v>
-      </c>
-      <c r="K3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -13212,7 +13224,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>

</xml_diff>

<commit_message>
General fixes and added indexing for wireframe of primary core in Show.py
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\Masters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F2BE5E-E663-459C-8C96-E00D06AA007F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358F2EC2-AB3D-45A5-9729-62647976CEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="0" windowWidth="14730" windowHeight="15600" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="2" r:id="rId1"/>
@@ -622,7 +622,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -695,6 +695,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -807,7 +814,7 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -866,6 +873,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -9937,25 +9947,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="7"/>
-    <col min="6" max="6" width="21.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="83.7109375" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="7"/>
+    <col min="4" max="4" width="23.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="7"/>
+    <col min="6" max="6" width="21.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="83.6640625" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -9981,7 +9991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -10006,7 +10016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -10030,7 +10040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -10054,7 +10064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -10078,7 +10088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -10104,7 +10114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -10128,7 +10138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -10152,7 +10162,7 @@
         <v>small source for error is sigma is not exact and rather is 1 or 0 which can be improved. I think we should comb through Grid class to make sure its mostly np.array not lists and clean it up</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -10176,7 +10186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -10200,7 +10210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -10224,7 +10234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -10248,7 +10258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -10272,7 +10282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -10296,7 +10306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -10320,7 +10330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
@@ -10346,7 +10356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
@@ -10370,7 +10380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -10394,7 +10404,7 @@
         <v>The worst case error is e^-17 and propogates to roughly e^-14 when calculating B field. This is still negligible</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -10420,7 +10430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
@@ -10444,7 +10454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
@@ -10468,7 +10478,7 @@
         <v>The worst case error is e^-17 and propogates to roughly e^-14 when calculating B field. This is still negligible</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -10492,7 +10502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
@@ -10516,7 +10526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>6</v>
       </c>
@@ -10540,7 +10550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>6</v>
       </c>
@@ -10564,7 +10574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>6</v>
       </c>
@@ -10588,7 +10598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>6</v>
       </c>
@@ -10612,7 +10622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>6</v>
       </c>
@@ -10636,7 +10646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
@@ -10660,7 +10670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
@@ -10684,7 +10694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
@@ -10710,7 +10720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>6</v>
       </c>
@@ -10734,7 +10744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>6</v>
       </c>
@@ -10758,7 +10768,7 @@
         <v>Assuming my math is right</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>6</v>
       </c>
@@ -10782,7 +10792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>6</v>
       </c>
@@ -10806,7 +10816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
@@ -10830,7 +10840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>6</v>
       </c>
@@ -10854,7 +10864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>6</v>
       </c>
@@ -10878,7 +10888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>6</v>
       </c>
@@ -10902,7 +10912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>6</v>
       </c>
@@ -10928,7 +10938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>6</v>
       </c>
@@ -10952,7 +10962,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>6</v>
       </c>
@@ -10976,7 +10986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>7</v>
       </c>
@@ -11002,7 +11012,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
@@ -11028,7 +11038,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
@@ -11054,7 +11064,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -11080,7 +11090,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -11106,7 +11116,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>7</v>
       </c>
@@ -11132,7 +11142,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
@@ -11158,7 +11168,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>7</v>
       </c>
@@ -11184,7 +11194,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>8</v>
       </c>
@@ -11210,7 +11220,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>8</v>
       </c>
@@ -11236,7 +11246,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>40</v>
       </c>
@@ -11262,7 +11272,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>40</v>
       </c>
@@ -11288,7 +11298,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>40</v>
       </c>
@@ -11314,7 +11324,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>40</v>
       </c>
@@ -11340,7 +11350,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B57" s="10" t="s">
         <v>45</v>
       </c>
@@ -11353,7 +11363,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>108</v>
       </c>
@@ -11368,10 +11378,10 @@
       </c>
       <c r="E58" s="15"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B59" s="7"/>
     </row>
-    <row r="60" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>107</v>
       </c>
@@ -11385,19 +11395,20 @@
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B61" s="7"/>
     </row>
-    <row r="62" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="s">
         <v>172</v>
       </c>
+      <c r="B62" s="22"/>
       <c r="C62" s="15"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
         <v>174</v>
       </c>
@@ -11408,10 +11419,10 @@
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B65" s="7"/>
     </row>
-    <row r="66" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>180</v>
       </c>
@@ -11422,12 +11433,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>181</v>
       </c>
@@ -11435,7 +11446,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>182</v>
       </c>
@@ -11458,13 +11469,13 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>95</v>
       </c>
@@ -11472,7 +11483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>67</v>
       </c>
@@ -11503,7 +11514,7 @@
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
     </row>
-    <row r="3" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>68</v>
       </c>
@@ -11540,7 +11551,7 @@
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
     </row>
-    <row r="4" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>69</v>
       </c>
@@ -11611,7 +11622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>70</v>
       </c>
@@ -11650,7 +11661,7 @@
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
     </row>
-    <row r="6" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>71</v>
       </c>
@@ -11697,7 +11708,7 @@
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
     </row>
-    <row r="7" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>72</v>
       </c>
@@ -11744,7 +11755,7 @@
       <c r="W7" s="8"/>
       <c r="X7" s="8"/>
     </row>
-    <row r="8" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>73</v>
       </c>
@@ -11779,7 +11790,7 @@
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
     </row>
-    <row r="9" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>74</v>
       </c>
@@ -11812,7 +11823,7 @@
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
     </row>
-    <row r="10" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>75</v>
       </c>
@@ -11855,7 +11866,7 @@
       <c r="W10" s="8"/>
       <c r="X10" s="8"/>
     </row>
-    <row r="11" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>76</v>
       </c>
@@ -11892,7 +11903,7 @@
       <c r="W11" s="8"/>
       <c r="X11" s="8"/>
     </row>
-    <row r="12" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>77</v>
       </c>
@@ -11900,7 +11911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>78</v>
       </c>
@@ -12295,7 +12306,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="14" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>79</v>
       </c>
@@ -12578,7 +12589,7 @@
       <c r="EA14" s="8"/>
       <c r="EB14" s="8"/>
     </row>
-    <row r="15" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>80</v>
       </c>
@@ -12586,7 +12597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:132" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>81</v>
       </c>
@@ -12594,7 +12605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>82</v>
       </c>
@@ -12602,7 +12613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>83</v>
       </c>
@@ -12610,7 +12621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>84</v>
       </c>
@@ -12618,7 +12629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>97</v>
       </c>
@@ -12626,7 +12637,7 @@
         <v>8640</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>98</v>
       </c>
@@ -12634,22 +12645,22 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>102</v>
       </c>
@@ -12667,15 +12678,15 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="16"/>
-    <col min="5" max="5" width="31.5703125" style="16" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="31.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.109375" style="16"/>
+    <col min="5" max="5" width="31.5546875" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>130</v>
       </c>
@@ -12692,7 +12703,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>131</v>
       </c>
@@ -12709,7 +12720,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>132</v>
       </c>
@@ -12723,7 +12734,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>133</v>
       </c>
@@ -12737,7 +12748,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>134</v>
       </c>
@@ -12751,7 +12762,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>135</v>
       </c>
@@ -12765,7 +12776,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>136</v>
       </c>
@@ -12779,7 +12790,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>137</v>
       </c>
@@ -12793,7 +12804,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>138</v>
       </c>
@@ -12807,7 +12818,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>139</v>
       </c>
@@ -12821,7 +12832,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>140</v>
       </c>
@@ -12835,7 +12846,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>141</v>
       </c>
@@ -12849,7 +12860,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>142</v>
       </c>
@@ -12863,7 +12874,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>143</v>
       </c>
@@ -12877,7 +12888,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>144</v>
       </c>
@@ -12891,7 +12902,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>146</v>
       </c>
@@ -12903,7 +12914,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>148</v>
       </c>
@@ -12915,7 +12926,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>145</v>
       </c>
@@ -12929,7 +12940,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>150</v>
       </c>
@@ -12943,7 +12954,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>151</v>
       </c>
@@ -12957,7 +12968,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>152</v>
       </c>
@@ -12971,7 +12982,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>170</v>
       </c>
@@ -12995,55 +13006,55 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="K2" s="22"/>
+      <c r="K2" s="23"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -13078,7 +13089,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6</v>
       </c>
@@ -13114,7 +13125,7 @@
         <v>-3.1E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8</v>
       </c>
@@ -13150,7 +13161,7 @@
         <v>-3.1E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10</v>
       </c>
@@ -13186,7 +13197,7 @@
         <v>-3.0499999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>12</v>
       </c>
@@ -13222,30 +13233,30 @@
         <v>-3.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Hx BC between MEC and HM should only have west and east MMF not westWest and eastEast
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358F2EC2-AB3D-45A5-9729-62647976CEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01378AC1-15C9-4212-8612-FBB2569825C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
+    <workbookView xWindow="-8508" yWindow="0" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="1" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="174">
   <si>
     <t>File</t>
   </si>
@@ -256,12 +256,6 @@
     <t>visualizeMatrix</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>If there is a * in the comment it means I have checked the method for different len(n) values and different mecRegionLengths</t>
-  </si>
-  <si>
     <t>ppAirBuffer</t>
   </si>
   <si>
@@ -356,18 +350,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>I am happy with everythin up until model.finalizeCompute</t>
-  </si>
-  <si>
-    <t>Anything inside finalizeCompute needs to be checked in debugger</t>
-  </si>
-  <si>
-    <t>Things like MMF, ur, sigma, Iph are not captured in the checkSpatialMapping and could be validated through a field plot using LIM_Show</t>
   </si>
   <si>
     <t>Assuming my math is right</t>
@@ -588,15 +570,6 @@
   </si>
   <si>
     <t>Check the Vect Pot around the upper 2 left coils</t>
-  </si>
-  <si>
-    <t>3) Look into other equations (hmMec)</t>
-  </si>
-  <si>
-    <t>2) Look at scalar potential after solving linalg near the coils and see where it tapers off using Show</t>
-  </si>
-  <si>
-    <t>4) Try to visualize the By BC between MEC and HM</t>
   </si>
   <si>
     <t>Visually draw on the Bx matplots markers where the upper and lower coils start</t>
@@ -622,7 +595,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -700,6 +673,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -814,7 +795,7 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -872,10 +853,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1109,10 +1093,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5300</c:v>
+                  <c:v>4900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1124,10 +1108,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5300</c:v>
+                  <c:v>4900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9945,10 +9929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10007,13 +9991,13 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G2" s="7" t="str">
-        <v>finalizeCompute</v>
+        <v>mecHm</v>
       </c>
       <c r="H2" s="7">
         <v>0</v>
       </c>
-      <c r="I2" s="7">
-        <v>0</v>
+      <c r="I2" s="7" t="str">
+        <v>The worst case error is e^-17 and propogates to roughly e^-14 when calculating B field. This is still negligible</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -10031,7 +10015,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G3" s="7" t="str">
-        <v>updateGrid</v>
+        <v>preEqn8</v>
       </c>
       <c r="H3" s="7">
         <v>0</v>
@@ -10052,16 +10036,16 @@
       </c>
       <c r="D4" s="2"/>
       <c r="F4" s="7" t="str">
-        <v>LIM_SlotPoleCalculation</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G4" s="7" t="str">
-        <v>LimMotor</v>
+        <v>eqn23Integral</v>
       </c>
       <c r="H4" s="7">
-        <v>100</v>
-      </c>
-      <c r="I4" s="7">
         <v>0</v>
+      </c>
+      <c r="I4" s="7" t="str">
+        <v>Assuming my math is right</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -10076,13 +10060,13 @@
       </c>
       <c r="D5" s="2"/>
       <c r="F5" s="7" t="str">
-        <v>LIM_SlotPoleCalculation</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G5" s="7" t="str">
-        <v>Error</v>
+        <v>buildMatAB</v>
       </c>
       <c r="H5" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I5" s="7">
         <v>0</v>
@@ -10102,13 +10086,13 @@
         <v>49</v>
       </c>
       <c r="F6" s="7" t="str">
-        <v>LIM_SlotPoleCalculation</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G6" s="7" t="str">
-        <v>np_find_nearest</v>
+        <v>finalizeCompute</v>
       </c>
       <c r="H6" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I6" s="7">
         <v>0</v>
@@ -10126,13 +10110,13 @@
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="7" t="str">
-        <v>LIM_SlotPoleCalculation</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G7" s="7" t="str">
-        <v>timing</v>
+        <v>updateGrid</v>
       </c>
       <c r="H7" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I7" s="7">
         <v>0</v>
@@ -10150,16 +10134,16 @@
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="7" t="str">
-        <v>LIM_Grid</v>
+        <v>LIM_SlotPoleCalculation</v>
       </c>
       <c r="G8" s="7" t="str">
-        <v>Grid</v>
+        <v>LimMotor</v>
       </c>
       <c r="H8" s="7">
         <v>100</v>
       </c>
-      <c r="I8" s="7" t="str">
-        <v>small source for error is sigma is not exact and rather is 1 or 0 which can be improved. I think we should comb through Grid class to make sure its mostly np.array not lists and clean it up</v>
+      <c r="I8" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -10174,10 +10158,10 @@
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="7" t="str">
-        <v>LIM_Grid</v>
+        <v>LIM_SlotPoleCalculation</v>
       </c>
       <c r="G9" s="7" t="str">
-        <v>Node</v>
+        <v>Error</v>
       </c>
       <c r="H9" s="7">
         <v>100</v>
@@ -10198,10 +10182,10 @@
       </c>
       <c r="D10" s="1"/>
       <c r="F10" s="7" t="str">
-        <v>LIM_Grid</v>
+        <v>LIM_SlotPoleCalculation</v>
       </c>
       <c r="G10" s="7" t="str">
-        <v>Region</v>
+        <v>np_find_nearest</v>
       </c>
       <c r="H10" s="7">
         <v>100</v>
@@ -10222,10 +10206,10 @@
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="7" t="str">
-        <v>LIM_Grid</v>
+        <v>LIM_SlotPoleCalculation</v>
       </c>
       <c r="G11" s="7" t="str">
-        <v>reluctance</v>
+        <v>timing</v>
       </c>
       <c r="H11" s="7">
         <v>100</v>
@@ -10249,13 +10233,13 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G12" s="7" t="str">
-        <v>meshBoundary</v>
+        <v>Grid</v>
       </c>
       <c r="H12" s="7">
         <v>100</v>
       </c>
-      <c r="I12" s="7">
-        <v>0</v>
+      <c r="I12" s="7" t="str">
+        <v>small source for error is sigma is not exact and rather is 1 or 0 which can be improved. I think we should comb through Grid class to make sure its mostly np.array not lists and clean it up</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -10273,7 +10257,7 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G13" s="7" t="str">
-        <v>checkSpatialMapping</v>
+        <v>Node</v>
       </c>
       <c r="H13" s="7">
         <v>100</v>
@@ -10297,7 +10281,7 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G14" s="7" t="str">
-        <v>buildGrid</v>
+        <v>Region</v>
       </c>
       <c r="H14" s="7">
         <v>100</v>
@@ -10321,7 +10305,7 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G15" s="7" t="str">
-        <v>setRegionIndices</v>
+        <v>reluctance</v>
       </c>
       <c r="H15" s="7">
         <v>100</v>
@@ -10341,13 +10325,13 @@
         <v>100</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F16" s="7" t="str">
         <v>LIM_Grid</v>
       </c>
       <c r="G16" s="7" t="str">
-        <v>finalizeGrid</v>
+        <v>meshBoundary</v>
       </c>
       <c r="H16" s="7">
         <v>100</v>
@@ -10363,15 +10347,15 @@
       <c r="B17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="23">
         <v>100</v>
       </c>
       <c r="D17" s="3"/>
       <c r="F17" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_Grid</v>
       </c>
       <c r="G17" s="7" t="str">
-        <v>Model</v>
+        <v>checkSpatialMapping</v>
       </c>
       <c r="H17" s="7">
         <v>100</v>
@@ -10380,7 +10364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -10392,16 +10376,16 @@
       </c>
       <c r="D18" s="3"/>
       <c r="F18" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_Grid</v>
       </c>
       <c r="G18" s="7" t="str">
-        <v>linalg_lu</v>
+        <v>buildGrid</v>
       </c>
       <c r="H18" s="7">
         <v>100</v>
       </c>
-      <c r="I18" s="7" t="str">
-        <v>The worst case error is e^-17 and propogates to roughly e^-14 when calculating B field. This is still negligible</v>
+      <c r="I18" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -10411,17 +10395,17 @@
       <c r="B19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="21">
-        <v>100</v>
+      <c r="C19" s="23">
+        <v>0</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F19" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_Grid</v>
       </c>
       <c r="G19" s="7" t="str">
-        <v>dirichlet</v>
+        <v>setRegionIndices</v>
       </c>
       <c r="H19" s="7">
         <v>100</v>
@@ -10437,15 +10421,15 @@
       <c r="B20" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="23">
         <v>100</v>
       </c>
       <c r="D20" s="3"/>
       <c r="F20" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_Grid</v>
       </c>
       <c r="G20" s="7" t="str">
-        <v>hmHm</v>
+        <v>finalizeGrid</v>
       </c>
       <c r="H20" s="7">
         <v>100</v>
@@ -10461,7 +10445,7 @@
       <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="23">
         <v>100</v>
       </c>
       <c r="D21" s="3"/>
@@ -10469,13 +10453,13 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G21" s="7" t="str">
-        <v>mecHm</v>
+        <v>Model</v>
       </c>
       <c r="H21" s="7">
         <v>100</v>
       </c>
-      <c r="I21" s="7" t="str">
-        <v>The worst case error is e^-17 and propogates to roughly e^-14 when calculating B field. This is still negligible</v>
+      <c r="I21" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -10485,7 +10469,7 @@
       <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="23">
         <v>100</v>
       </c>
       <c r="D22" s="3"/>
@@ -10493,13 +10477,13 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G22" s="7" t="str">
-        <v>mec</v>
+        <v>linalg_lu</v>
       </c>
       <c r="H22" s="7">
         <v>100</v>
       </c>
-      <c r="I22" s="7">
-        <v>0</v>
+      <c r="I22" s="7" t="str">
+        <v>The worst case error is e^-17 and propogates to roughly e^-14 when calculating B field. This is still negligible</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -10509,7 +10493,7 @@
       <c r="B23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="23">
         <v>100</v>
       </c>
       <c r="D23" s="3"/>
@@ -10517,7 +10501,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G23" s="7" t="str">
-        <v>preEqn24_2018</v>
+        <v>dirichlet</v>
       </c>
       <c r="H23" s="7">
         <v>100</v>
@@ -10534,14 +10518,14 @@
         <v>22</v>
       </c>
       <c r="C24" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D24" s="3"/>
       <c r="F24" s="7" t="str">
         <v>LIM_Compute</v>
       </c>
       <c r="G24" s="7" t="str">
-        <v>preEqn25_2018</v>
+        <v>hmHm</v>
       </c>
       <c r="H24" s="7">
         <v>100</v>
@@ -10557,7 +10541,7 @@
       <c r="B25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="23">
         <v>100</v>
       </c>
       <c r="D25" s="3"/>
@@ -10565,7 +10549,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G25" s="7" t="str">
-        <v>postMECAvgB</v>
+        <v>mec</v>
       </c>
       <c r="H25" s="7">
         <v>100</v>
@@ -10581,7 +10565,7 @@
       <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="23">
         <v>100</v>
       </c>
       <c r="D26" s="3"/>
@@ -10589,7 +10573,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G26" s="7" t="str">
-        <v>preEqn8</v>
+        <v>preEqn24_2018</v>
       </c>
       <c r="H26" s="7">
         <v>100</v>
@@ -10605,7 +10589,7 @@
       <c r="B27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="23">
         <v>100</v>
       </c>
       <c r="D27" s="3"/>
@@ -10613,7 +10597,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G27" s="7" t="str">
-        <v>postEqn8</v>
+        <v>preEqn25_2018</v>
       </c>
       <c r="H27" s="7">
         <v>100</v>
@@ -10629,7 +10613,7 @@
       <c r="B28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="23">
         <v>100</v>
       </c>
       <c r="D28" s="3"/>
@@ -10637,7 +10621,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G28" s="7" t="str">
-        <v>postEqn9</v>
+        <v>postMECAvgB</v>
       </c>
       <c r="H28" s="7">
         <v>100</v>
@@ -10661,7 +10645,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G29" s="7" t="str">
-        <v>postEqn14to15</v>
+        <v>postEqn8</v>
       </c>
       <c r="H29" s="7">
         <v>100</v>
@@ -10685,7 +10669,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G30" s="7" t="str">
-        <v>postEqn16to17</v>
+        <v>postEqn9</v>
       </c>
       <c r="H30" s="7">
         <v>100</v>
@@ -10702,16 +10686,16 @@
         <v>29</v>
       </c>
       <c r="C31" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F31" s="7" t="str">
         <v>LIM_Compute</v>
       </c>
       <c r="G31" s="7" t="str">
-        <v>preEqn21</v>
+        <v>postEqn14to15</v>
       </c>
       <c r="H31" s="7">
         <v>100</v>
@@ -10735,7 +10719,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G32" s="7" t="str">
-        <v>postEqn21</v>
+        <v>postEqn16to17</v>
       </c>
       <c r="H32" s="7">
         <v>100</v>
@@ -10759,13 +10743,13 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G33" s="7" t="str">
-        <v>eqn23Integral</v>
+        <v>preEqn21</v>
       </c>
       <c r="H33" s="7">
         <v>100</v>
       </c>
-      <c r="I33" s="7" t="str">
-        <v>Assuming my math is right</v>
+      <c r="I33" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -10783,7 +10767,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G34" s="7" t="str">
-        <v>checkForErrors</v>
+        <v>postEqn21</v>
       </c>
       <c r="H34" s="7">
         <v>100</v>
@@ -10807,7 +10791,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G35" s="7" t="str">
-        <v>neighbourNodes</v>
+        <v>checkForErrors</v>
       </c>
       <c r="H35" s="7">
         <v>100</v>
@@ -10824,14 +10808,14 @@
         <v>31</v>
       </c>
       <c r="C36" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D36" s="3"/>
       <c r="F36" s="7" t="str">
         <v>LIM_Compute</v>
       </c>
       <c r="G36" s="7" t="str">
-        <v>boundaryInfo</v>
+        <v>neighbourNodes</v>
       </c>
       <c r="H36" s="7">
         <v>100</v>
@@ -10855,7 +10839,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G37" s="7" t="str">
-        <v>reduceMatrix</v>
+        <v>boundaryInfo</v>
       </c>
       <c r="H37" s="7">
         <v>100</v>
@@ -10879,7 +10863,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G38" s="7" t="str">
-        <v>buildMatAB</v>
+        <v>reduceMatrix</v>
       </c>
       <c r="H38" s="7">
         <v>100</v>
@@ -10922,9 +10906,7 @@
       <c r="C40" s="3">
         <v>100</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="D40" s="3"/>
       <c r="F40" s="7" t="str">
         <v>LIM_Compute</v>
       </c>
@@ -10958,8 +10940,8 @@
       <c r="H41" s="7">
         <v>100</v>
       </c>
-      <c r="I41" s="7" t="str">
-        <v>*</v>
+      <c r="I41" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -10996,9 +10978,7 @@
       <c r="C43" s="4">
         <v>100</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="D43" s="4"/>
       <c r="F43" s="7" t="str">
         <v>LIM_Show</v>
       </c>
@@ -11008,8 +10988,8 @@
       <c r="H43" s="7">
         <v>100</v>
       </c>
-      <c r="I43" s="7" t="str">
-        <v>*</v>
+      <c r="I43" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -11022,9 +11002,7 @@
       <c r="C44" s="4">
         <v>100</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="D44" s="4"/>
       <c r="F44" s="7" t="str">
         <v>LIM_Show</v>
       </c>
@@ -11034,8 +11012,8 @@
       <c r="H44" s="7">
         <v>100</v>
       </c>
-      <c r="I44" s="7" t="str">
-        <v>*</v>
+      <c r="I44" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -11048,9 +11026,7 @@
       <c r="C45" s="4">
         <v>100</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="D45" s="4"/>
       <c r="F45" s="7" t="str">
         <v>LIM_Show</v>
       </c>
@@ -11060,8 +11036,8 @@
       <c r="H45" s="7">
         <v>100</v>
       </c>
-      <c r="I45" s="7" t="str">
-        <v>*</v>
+      <c r="I45" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -11074,9 +11050,7 @@
       <c r="C46" s="4">
         <v>100</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="D46" s="4"/>
       <c r="F46" s="7" t="str">
         <v>LIM_Show</v>
       </c>
@@ -11086,8 +11060,8 @@
       <c r="H46" s="7">
         <v>100</v>
       </c>
-      <c r="I46" s="7" t="str">
-        <v>*</v>
+      <c r="I46" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -11100,9 +11074,7 @@
       <c r="C47" s="4">
         <v>100</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="D47" s="4"/>
       <c r="F47" s="7" t="str">
         <v>LIM_Show</v>
       </c>
@@ -11112,8 +11084,8 @@
       <c r="H47" s="7">
         <v>100</v>
       </c>
-      <c r="I47" s="7" t="str">
-        <v>*</v>
+      <c r="I47" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -11126,9 +11098,7 @@
       <c r="C48" s="4">
         <v>100</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="D48" s="4"/>
       <c r="F48" s="7" t="str">
         <v>LIM_Show</v>
       </c>
@@ -11138,8 +11108,8 @@
       <c r="H48" s="7">
         <v>100</v>
       </c>
-      <c r="I48" s="7" t="str">
-        <v>*</v>
+      <c r="I48" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -11152,9 +11122,7 @@
       <c r="C49" s="4">
         <v>100</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="D49" s="4"/>
       <c r="F49" s="7" t="str">
         <v>LIM_Show</v>
       </c>
@@ -11164,8 +11132,8 @@
       <c r="H49" s="7">
         <v>100</v>
       </c>
-      <c r="I49" s="7" t="str">
-        <v>*</v>
+      <c r="I49" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -11178,9 +11146,7 @@
       <c r="C50" s="4">
         <v>100</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="D50" s="4"/>
       <c r="F50" s="7" t="str">
         <v>LIM_Show</v>
       </c>
@@ -11190,8 +11156,8 @@
       <c r="H50" s="7">
         <v>100</v>
       </c>
-      <c r="I50" s="7" t="str">
-        <v>*</v>
+      <c r="I50" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -11204,9 +11170,7 @@
       <c r="C51" s="5">
         <v>100</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="D51" s="5"/>
       <c r="F51" s="7" t="str">
         <v>LIM_ShowFromJSON</v>
       </c>
@@ -11216,8 +11180,8 @@
       <c r="H51" s="7">
         <v>100</v>
       </c>
-      <c r="I51" s="7" t="str">
-        <v>*</v>
+      <c r="I51" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -11230,9 +11194,7 @@
       <c r="C52" s="5">
         <v>100</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="D52" s="5"/>
       <c r="F52" s="7" t="str">
         <v>LIM_ShowFromJSON</v>
       </c>
@@ -11242,8 +11204,8 @@
       <c r="H52" s="7">
         <v>100</v>
       </c>
-      <c r="I52" s="7" t="str">
-        <v>*</v>
+      <c r="I52" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -11256,9 +11218,7 @@
       <c r="C53" s="6">
         <v>100</v>
       </c>
-      <c r="D53" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="D53" s="6"/>
       <c r="F53" s="7" t="str">
         <v>Platypus</v>
       </c>
@@ -11268,8 +11228,8 @@
       <c r="H53" s="7">
         <v>100</v>
       </c>
-      <c r="I53" s="7" t="str">
-        <v>*</v>
+      <c r="I53" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -11282,9 +11242,7 @@
       <c r="C54" s="6">
         <v>100</v>
       </c>
-      <c r="D54" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="D54" s="6"/>
       <c r="F54" s="7" t="str">
         <v>Platypus</v>
       </c>
@@ -11294,8 +11252,8 @@
       <c r="H54" s="7">
         <v>100</v>
       </c>
-      <c r="I54" s="7" t="str">
-        <v>*</v>
+      <c r="I54" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -11308,9 +11266,7 @@
       <c r="C55" s="6">
         <v>100</v>
       </c>
-      <c r="D55" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="D55" s="6"/>
       <c r="F55" s="7" t="str">
         <v>Platypus</v>
       </c>
@@ -11320,8 +11276,8 @@
       <c r="H55" s="7">
         <v>100</v>
       </c>
-      <c r="I55" s="7" t="str">
-        <v>*</v>
+      <c r="I55" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -11334,9 +11290,7 @@
       <c r="C56" s="6">
         <v>100</v>
       </c>
-      <c r="D56" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="D56" s="6"/>
       <c r="F56" s="7" t="str">
         <v>Platypus</v>
       </c>
@@ -11346,8 +11300,8 @@
       <c r="H56" s="7">
         <v>100</v>
       </c>
-      <c r="I56" s="7" t="str">
-        <v>*</v>
+      <c r="I56" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -11356,25 +11310,22 @@
       </c>
       <c r="C57" s="7">
         <f>SUM(TrackIssues5[Confidence])</f>
-        <v>5300</v>
+        <v>4900</v>
       </c>
       <c r="D57" s="7">
         <f>ROWS(TrackIssues5[Confidence]) *100 - C57</f>
-        <v>200</v>
+        <v>600</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="E58" s="15"/>
     </row>
@@ -11383,16 +11334,16 @@
     </row>
     <row r="60" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -11400,9 +11351,9 @@
     </row>
     <row r="62" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="B62" s="22"/>
+        <v>166</v>
+      </c>
+      <c r="B62" s="21"/>
       <c r="C62" s="15"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -11410,46 +11361,34 @@
     </row>
     <row r="64" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B65" s="7"/>
     </row>
-    <row r="66" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>176</v>
+        <v>171</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>170</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A67" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="7" t="s">
-        <v>182</v>
-      </c>
+    <row r="68" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="B68" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11463,10 +11402,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB53FA3-97E7-4737-912B-B0A83665D811}">
-  <dimension ref="A1:EB26"/>
+  <dimension ref="A1:AZ21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11475,23 +11414,23 @@
     <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:132" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" s="9">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:132" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="8">
-        <v>116</v>
+        <v>40</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -11514,25 +11453,21 @@
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
     </row>
-    <row r="3" spans="1:132" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
       </c>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8">
-        <v>2</v>
-      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -11551,100 +11486,72 @@
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
     </row>
-    <row r="4" spans="1:132" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>63</v>
       </c>
       <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>2</v>
+      </c>
+      <c r="G4" s="8">
         <v>3</v>
       </c>
-      <c r="F4" s="8">
+      <c r="H4" s="8">
         <v>4</v>
       </c>
-      <c r="G4" s="8">
+      <c r="I4" s="8">
         <v>5</v>
       </c>
-      <c r="H4" s="8">
+      <c r="J4" s="8">
         <v>6</v>
       </c>
-      <c r="I4" s="8">
+      <c r="K4" s="8">
         <v>7</v>
       </c>
-      <c r="J4" s="8">
+      <c r="L4" s="8">
         <v>8</v>
       </c>
-      <c r="K4" s="8">
-        <v>9</v>
-      </c>
-      <c r="L4" s="8">
-        <v>10</v>
-      </c>
-      <c r="M4" s="8">
-        <v>11</v>
-      </c>
-      <c r="N4" s="8">
-        <v>12</v>
-      </c>
-      <c r="O4" s="8">
-        <v>13</v>
-      </c>
-      <c r="P4" s="8">
-        <v>14</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>15</v>
-      </c>
-      <c r="R4" s="8">
-        <v>16</v>
-      </c>
-      <c r="S4" s="8">
-        <v>17</v>
-      </c>
-      <c r="T4" s="8">
-        <v>18</v>
-      </c>
-      <c r="U4" s="8">
-        <v>19</v>
-      </c>
-      <c r="V4" s="8">
-        <v>20</v>
-      </c>
-      <c r="W4" s="8">
-        <v>21</v>
-      </c>
-      <c r="X4" s="8">
-        <v>22</v>
-      </c>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
     </row>
-    <row r="5" spans="1:132" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" s="8">
         <v>1</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
-        <v>91</v>
+      <c r="D5" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
       </c>
       <c r="F5" s="8">
-        <v>3</v>
-      </c>
-      <c r="G5" s="8">
-        <v>4</v>
-      </c>
-      <c r="H5" s="8">
-        <v>5</v>
-      </c>
-      <c r="I5" s="8">
-        <v>6</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
@@ -11661,41 +11568,31 @@
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
     </row>
-    <row r="6" spans="1:132" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="8">
-        <v>35</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8" t="s">
-        <v>92</v>
+        <v>14</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="8">
+        <v>3</v>
       </c>
       <c r="F6" s="8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G6" s="8">
-        <v>8</v>
-      </c>
-      <c r="H6" s="8">
-        <v>9</v>
-      </c>
-      <c r="I6" s="8">
-        <v>10</v>
-      </c>
-      <c r="J6" s="8">
-        <v>11</v>
-      </c>
-      <c r="K6" s="8">
-        <v>12</v>
-      </c>
-      <c r="L6" s="8">
-        <v>13</v>
-      </c>
-      <c r="M6" s="8">
-        <v>14</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
@@ -11708,41 +11605,31 @@
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
     </row>
-    <row r="7" spans="1:132" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B7" s="8">
-        <v>20</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
-        <v>93</v>
+        <v>8</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="8">
+        <v>6</v>
       </c>
       <c r="F7" s="8">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G7" s="8">
-        <v>16</v>
-      </c>
-      <c r="H7" s="8">
-        <v>17</v>
-      </c>
-      <c r="I7" s="8">
-        <v>18</v>
-      </c>
-      <c r="J7" s="8">
-        <v>19</v>
-      </c>
-      <c r="K7" s="8">
-        <v>20</v>
-      </c>
-      <c r="L7" s="8">
-        <v>21</v>
-      </c>
-      <c r="M7" s="8">
-        <v>22</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
@@ -11755,22 +11642,20 @@
       <c r="W7" s="8"/>
       <c r="X7" s="8"/>
     </row>
-    <row r="8" spans="1:132" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" s="8">
-        <v>432</v>
+        <v>164</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" s="8">
-        <v>23</v>
-      </c>
-      <c r="F8" s="8">
-        <v>24</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -11790,18 +11675,18 @@
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
     </row>
-    <row r="9" spans="1:132" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B9" s="8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E9" s="8">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -11823,34 +11708,26 @@
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
     </row>
-    <row r="10" spans="1:132" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10" s="8">
-        <v>432</v>
+        <v>164</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E10" s="8">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F10" s="8">
-        <v>27</v>
-      </c>
-      <c r="G10" s="8">
-        <v>28</v>
-      </c>
-      <c r="H10" s="8">
-        <v>29</v>
-      </c>
-      <c r="I10" s="8">
-        <v>30</v>
-      </c>
-      <c r="J10" s="8">
-        <v>31</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
@@ -11866,25 +11743,21 @@
       <c r="W10" s="8"/>
       <c r="X10" s="8"/>
     </row>
-    <row r="11" spans="1:132" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B11" s="8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E11" s="8">
-        <v>32</v>
-      </c>
-      <c r="F11" s="8">
-        <v>33</v>
-      </c>
-      <c r="G11" s="8">
-        <v>34</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -11903,727 +11776,335 @@
       <c r="W11" s="8"/>
       <c r="X11" s="8"/>
     </row>
-    <row r="12" spans="1:132" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="8">
+        <v>6</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="8">
+        <v>43</v>
+      </c>
+      <c r="F13" s="8">
+        <v>44</v>
+      </c>
+      <c r="G13" s="8">
+        <v>45</v>
+      </c>
+      <c r="H13" s="8">
+        <v>48</v>
+      </c>
+      <c r="I13" s="8">
+        <v>49</v>
+      </c>
+      <c r="J13" s="8">
+        <v>50</v>
+      </c>
+      <c r="K13" s="8">
+        <v>53</v>
+      </c>
+      <c r="L13" s="8">
+        <v>54</v>
+      </c>
+      <c r="M13" s="8">
+        <v>55</v>
+      </c>
+      <c r="N13" s="8">
+        <v>58</v>
+      </c>
+      <c r="O13" s="8">
+        <v>59</v>
+      </c>
+      <c r="P13" s="8">
+        <v>60</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>63</v>
+      </c>
+      <c r="R13" s="8">
+        <v>64</v>
+      </c>
+      <c r="S13" s="8">
+        <v>65</v>
+      </c>
+      <c r="T13" s="8">
+        <v>68</v>
+      </c>
+      <c r="U13" s="8">
+        <v>69</v>
+      </c>
+      <c r="V13" s="8">
+        <v>70</v>
+      </c>
+      <c r="W13" s="8">
+        <v>73</v>
+      </c>
+      <c r="X13" s="8">
+        <v>74</v>
+      </c>
+      <c r="Y13" s="8">
+        <v>75</v>
+      </c>
+      <c r="Z13" s="8">
+        <v>78</v>
+      </c>
+      <c r="AA13" s="8">
+        <v>79</v>
+      </c>
+      <c r="AB13" s="8">
+        <v>80</v>
+      </c>
+      <c r="AC13" s="8">
+        <v>83</v>
+      </c>
+      <c r="AD13" s="8">
+        <v>84</v>
+      </c>
+      <c r="AE13" s="8">
+        <v>85</v>
+      </c>
+      <c r="AF13" s="8">
+        <v>88</v>
+      </c>
+      <c r="AG13" s="8">
+        <v>89</v>
+      </c>
+      <c r="AH13" s="8">
+        <v>90</v>
+      </c>
+      <c r="AI13" s="8">
+        <v>93</v>
+      </c>
+      <c r="AJ13" s="8">
+        <v>94</v>
+      </c>
+      <c r="AK13" s="8">
+        <v>95</v>
+      </c>
+      <c r="AL13" s="8">
+        <v>98</v>
+      </c>
+      <c r="AM13" s="8">
+        <v>99</v>
+      </c>
+      <c r="AN13" s="8">
+        <v>100</v>
+      </c>
+      <c r="AO13" s="8">
+        <v>103</v>
+      </c>
+      <c r="AP13" s="8">
+        <v>104</v>
+      </c>
+      <c r="AQ13" s="8">
+        <v>105</v>
+      </c>
+      <c r="AR13" s="8">
+        <v>108</v>
+      </c>
+      <c r="AS13" s="8">
+        <v>109</v>
+      </c>
+      <c r="AT13" s="8">
+        <v>110</v>
+      </c>
+      <c r="AU13" s="8">
+        <v>113</v>
+      </c>
+      <c r="AV13" s="8">
+        <v>114</v>
+      </c>
+      <c r="AW13" s="8">
+        <v>115</v>
+      </c>
+      <c r="AX13" s="8">
+        <v>118</v>
+      </c>
+      <c r="AY13" s="8">
+        <v>119</v>
+      </c>
+      <c r="AZ13" s="8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="8">
-        <v>8</v>
-      </c>
+      <c r="B14" s="8">
+        <v>5</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="8">
+        <v>40</v>
+      </c>
+      <c r="F14" s="8">
+        <v>41</v>
+      </c>
+      <c r="G14" s="8">
+        <v>42</v>
+      </c>
+      <c r="H14" s="8">
+        <v>46</v>
+      </c>
+      <c r="I14" s="8">
+        <v>47</v>
+      </c>
+      <c r="J14" s="8">
+        <v>51</v>
+      </c>
+      <c r="K14" s="8">
+        <v>52</v>
+      </c>
+      <c r="L14" s="8">
+        <v>56</v>
+      </c>
+      <c r="M14" s="8">
+        <v>57</v>
+      </c>
+      <c r="N14" s="8">
+        <v>61</v>
+      </c>
+      <c r="O14" s="8">
+        <v>62</v>
+      </c>
+      <c r="P14" s="8">
+        <v>66</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>67</v>
+      </c>
+      <c r="R14" s="8">
+        <v>71</v>
+      </c>
+      <c r="S14" s="8">
+        <v>72</v>
+      </c>
+      <c r="T14" s="8">
+        <v>76</v>
+      </c>
+      <c r="U14" s="8">
+        <v>77</v>
+      </c>
+      <c r="V14" s="8">
+        <v>81</v>
+      </c>
+      <c r="W14" s="8">
+        <v>82</v>
+      </c>
+      <c r="X14" s="8">
+        <v>86</v>
+      </c>
+      <c r="Y14" s="8">
+        <v>87</v>
+      </c>
+      <c r="Z14" s="8">
+        <v>91</v>
+      </c>
+      <c r="AA14" s="8">
+        <v>92</v>
+      </c>
+      <c r="AB14" s="8">
+        <v>96</v>
+      </c>
+      <c r="AC14" s="8">
+        <v>97</v>
+      </c>
+      <c r="AD14" s="8">
+        <v>101</v>
+      </c>
+      <c r="AE14" s="8">
+        <v>102</v>
+      </c>
+      <c r="AF14" s="8">
+        <v>106</v>
+      </c>
+      <c r="AG14" s="8">
+        <v>107</v>
+      </c>
+      <c r="AH14" s="8">
+        <v>111</v>
+      </c>
+      <c r="AI14" s="8">
+        <v>112</v>
+      </c>
+      <c r="AJ14" s="8">
+        <v>116</v>
+      </c>
+      <c r="AK14" s="8">
+        <v>117</v>
+      </c>
+      <c r="AL14" s="8">
+        <v>121</v>
+      </c>
+      <c r="AM14" s="8">
+        <v>122</v>
+      </c>
+      <c r="AN14" s="8">
+        <v>123</v>
+      </c>
+      <c r="AO14" s="8"/>
+      <c r="AP14" s="8"/>
+      <c r="AQ14" s="8"/>
+      <c r="AR14" s="8"/>
+      <c r="AS14" s="8"/>
+      <c r="AT14" s="8"/>
+      <c r="AU14" s="8"/>
+      <c r="AV14" s="8"/>
+      <c r="AW14" s="8"/>
+      <c r="AX14" s="8"/>
+      <c r="AY14" s="8"/>
+      <c r="AZ14" s="8"/>
     </row>
-    <row r="13" spans="1:132" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="8">
-        <v>16</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="8">
-        <v>122</v>
-      </c>
-      <c r="F13" s="8">
-        <v>123</v>
-      </c>
-      <c r="G13" s="8">
-        <v>124</v>
-      </c>
-      <c r="H13" s="8">
-        <v>125</v>
-      </c>
-      <c r="I13" s="8">
-        <v>126</v>
-      </c>
-      <c r="J13" s="8">
-        <v>127</v>
-      </c>
-      <c r="K13" s="8">
-        <v>128</v>
-      </c>
-      <c r="L13" s="8">
-        <v>129</v>
-      </c>
-      <c r="M13" s="8">
-        <v>134</v>
-      </c>
-      <c r="N13" s="8">
-        <v>135</v>
-      </c>
-      <c r="O13" s="8">
-        <v>136</v>
-      </c>
-      <c r="P13" s="8">
-        <v>137</v>
-      </c>
-      <c r="Q13" s="8">
-        <v>138</v>
-      </c>
-      <c r="R13" s="8">
-        <v>139</v>
-      </c>
-      <c r="S13" s="8">
-        <v>140</v>
-      </c>
-      <c r="T13" s="8">
-        <v>141</v>
-      </c>
-      <c r="U13" s="8">
-        <v>146</v>
-      </c>
-      <c r="V13" s="8">
-        <v>147</v>
-      </c>
-      <c r="W13" s="8">
-        <v>148</v>
-      </c>
-      <c r="X13" s="8">
-        <v>149</v>
-      </c>
-      <c r="Y13" s="8">
-        <v>150</v>
-      </c>
-      <c r="Z13" s="8">
-        <v>151</v>
-      </c>
-      <c r="AA13" s="8">
-        <v>152</v>
-      </c>
-      <c r="AB13" s="8">
-        <v>153</v>
-      </c>
-      <c r="AC13" s="8">
-        <v>158</v>
-      </c>
-      <c r="AD13" s="8">
-        <v>159</v>
-      </c>
-      <c r="AE13" s="8">
-        <v>160</v>
-      </c>
-      <c r="AF13" s="8">
-        <v>161</v>
-      </c>
-      <c r="AG13" s="8">
-        <v>162</v>
-      </c>
-      <c r="AH13" s="8">
-        <v>163</v>
-      </c>
-      <c r="AI13" s="8">
-        <v>164</v>
-      </c>
-      <c r="AJ13" s="8">
-        <v>165</v>
-      </c>
-      <c r="AK13" s="8">
-        <v>170</v>
-      </c>
-      <c r="AL13" s="8">
-        <v>171</v>
-      </c>
-      <c r="AM13" s="8">
-        <v>172</v>
-      </c>
-      <c r="AN13" s="8">
-        <v>173</v>
-      </c>
-      <c r="AO13" s="8">
-        <v>174</v>
-      </c>
-      <c r="AP13" s="8">
-        <v>175</v>
-      </c>
-      <c r="AQ13" s="8">
-        <v>176</v>
-      </c>
-      <c r="AR13" s="8">
-        <v>177</v>
-      </c>
-      <c r="AS13" s="8">
-        <v>182</v>
-      </c>
-      <c r="AT13" s="8">
-        <v>183</v>
-      </c>
-      <c r="AU13" s="8">
-        <v>184</v>
-      </c>
-      <c r="AV13" s="8">
-        <v>185</v>
-      </c>
-      <c r="AW13" s="8">
-        <v>186</v>
-      </c>
-      <c r="AX13" s="8">
-        <v>187</v>
-      </c>
-      <c r="AY13" s="8">
-        <v>188</v>
-      </c>
-      <c r="AZ13" s="8">
-        <v>189</v>
-      </c>
-      <c r="BA13" s="8">
-        <v>194</v>
-      </c>
-      <c r="BB13" s="8">
-        <v>195</v>
-      </c>
-      <c r="BC13" s="8">
-        <v>196</v>
-      </c>
-      <c r="BD13" s="8">
-        <v>197</v>
-      </c>
-      <c r="BE13" s="8">
-        <v>198</v>
-      </c>
-      <c r="BF13" s="8">
-        <v>199</v>
-      </c>
-      <c r="BG13" s="8">
-        <v>200</v>
-      </c>
-      <c r="BH13" s="8">
-        <v>201</v>
-      </c>
-      <c r="BI13" s="8">
-        <v>206</v>
-      </c>
-      <c r="BJ13" s="8">
-        <v>207</v>
-      </c>
-      <c r="BK13" s="8">
-        <v>208</v>
-      </c>
-      <c r="BL13" s="8">
-        <v>209</v>
-      </c>
-      <c r="BM13" s="8">
-        <v>210</v>
-      </c>
-      <c r="BN13" s="8">
-        <v>211</v>
-      </c>
-      <c r="BO13" s="8">
-        <v>212</v>
-      </c>
-      <c r="BP13" s="8">
-        <v>213</v>
-      </c>
-      <c r="BQ13" s="8">
-        <v>218</v>
-      </c>
-      <c r="BR13" s="8">
-        <v>219</v>
-      </c>
-      <c r="BS13" s="8">
-        <v>220</v>
-      </c>
-      <c r="BT13" s="8">
-        <v>221</v>
-      </c>
-      <c r="BU13" s="8">
-        <v>222</v>
-      </c>
-      <c r="BV13" s="8">
-        <v>223</v>
-      </c>
-      <c r="BW13" s="8">
-        <v>224</v>
-      </c>
-      <c r="BX13" s="8">
-        <v>225</v>
-      </c>
-      <c r="BY13" s="8">
-        <v>230</v>
-      </c>
-      <c r="BZ13" s="8">
-        <v>231</v>
-      </c>
-      <c r="CA13" s="8">
-        <v>232</v>
-      </c>
-      <c r="CB13" s="8">
-        <v>233</v>
-      </c>
-      <c r="CC13" s="8">
-        <v>234</v>
-      </c>
-      <c r="CD13" s="8">
-        <v>235</v>
-      </c>
-      <c r="CE13" s="8">
-        <v>236</v>
-      </c>
-      <c r="CF13" s="8">
-        <v>237</v>
-      </c>
-      <c r="CG13" s="8">
-        <v>242</v>
-      </c>
-      <c r="CH13" s="8">
-        <v>243</v>
-      </c>
-      <c r="CI13" s="8">
-        <v>244</v>
-      </c>
-      <c r="CJ13" s="8">
-        <v>245</v>
-      </c>
-      <c r="CK13" s="8">
-        <v>246</v>
-      </c>
-      <c r="CL13" s="8">
-        <v>247</v>
-      </c>
-      <c r="CM13" s="8">
-        <v>248</v>
-      </c>
-      <c r="CN13" s="8">
-        <v>249</v>
-      </c>
-      <c r="CO13" s="8">
-        <v>254</v>
-      </c>
-      <c r="CP13" s="8">
-        <v>255</v>
-      </c>
-      <c r="CQ13" s="8">
-        <v>256</v>
-      </c>
-      <c r="CR13" s="8">
-        <v>257</v>
-      </c>
-      <c r="CS13" s="8">
-        <v>258</v>
-      </c>
-      <c r="CT13" s="8">
-        <v>259</v>
-      </c>
-      <c r="CU13" s="8">
-        <v>260</v>
-      </c>
-      <c r="CV13" s="8">
-        <v>261</v>
-      </c>
-      <c r="CW13" s="8">
-        <v>266</v>
-      </c>
-      <c r="CX13" s="8">
-        <v>267</v>
-      </c>
-      <c r="CY13" s="8">
-        <v>268</v>
-      </c>
-      <c r="CZ13" s="8">
-        <v>269</v>
-      </c>
-      <c r="DA13" s="8">
-        <v>270</v>
-      </c>
-      <c r="DB13" s="8">
-        <v>271</v>
-      </c>
-      <c r="DC13" s="8">
-        <v>272</v>
-      </c>
-      <c r="DD13" s="8">
-        <v>273</v>
-      </c>
-      <c r="DE13" s="8">
-        <v>278</v>
-      </c>
-      <c r="DF13" s="8">
-        <v>279</v>
-      </c>
-      <c r="DG13" s="8">
-        <v>280</v>
-      </c>
-      <c r="DH13" s="8">
-        <v>281</v>
-      </c>
-      <c r="DI13" s="8">
-        <v>282</v>
-      </c>
-      <c r="DJ13" s="8">
-        <v>283</v>
-      </c>
-      <c r="DK13" s="8">
-        <v>284</v>
-      </c>
-      <c r="DL13" s="8">
-        <v>285</v>
-      </c>
-      <c r="DM13" s="8">
-        <v>290</v>
-      </c>
-      <c r="DN13" s="8">
-        <v>291</v>
-      </c>
-      <c r="DO13" s="8">
-        <v>292</v>
-      </c>
-      <c r="DP13" s="8">
-        <v>293</v>
-      </c>
-      <c r="DQ13" s="8">
-        <v>294</v>
-      </c>
-      <c r="DR13" s="8">
-        <v>295</v>
-      </c>
-      <c r="DS13" s="8">
-        <v>296</v>
-      </c>
-      <c r="DT13" s="8">
-        <v>297</v>
-      </c>
-      <c r="DU13" s="8">
-        <v>302</v>
-      </c>
-      <c r="DV13" s="8">
-        <v>303</v>
-      </c>
-      <c r="DW13" s="8">
-        <v>304</v>
-      </c>
-      <c r="DX13" s="8">
-        <v>305</v>
-      </c>
-      <c r="DY13" s="8">
-        <v>306</v>
-      </c>
-      <c r="DZ13" s="8">
-        <v>307</v>
-      </c>
-      <c r="EA13" s="8">
-        <v>308</v>
-      </c>
-      <c r="EB13" s="8">
-        <v>309</v>
+      <c r="B15" s="8">
+        <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:132" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="8">
-        <v>12</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="8">
-        <v>116</v>
-      </c>
-      <c r="F14" s="8">
-        <v>117</v>
-      </c>
-      <c r="G14" s="8">
-        <v>118</v>
-      </c>
-      <c r="H14" s="8">
-        <v>119</v>
-      </c>
-      <c r="I14" s="8">
-        <v>120</v>
-      </c>
-      <c r="J14" s="8">
-        <v>121</v>
-      </c>
-      <c r="K14" s="8">
-        <v>130</v>
-      </c>
-      <c r="L14" s="8">
-        <v>131</v>
-      </c>
-      <c r="M14" s="8">
-        <v>132</v>
-      </c>
-      <c r="N14" s="8">
-        <v>133</v>
-      </c>
-      <c r="O14" s="8">
-        <v>142</v>
-      </c>
-      <c r="P14" s="8">
-        <v>143</v>
-      </c>
-      <c r="Q14" s="8">
-        <v>144</v>
-      </c>
-      <c r="R14" s="8">
-        <v>145</v>
-      </c>
-      <c r="S14" s="8">
-        <v>154</v>
-      </c>
-      <c r="T14" s="8">
-        <v>155</v>
-      </c>
-      <c r="U14" s="8">
-        <v>156</v>
-      </c>
-      <c r="V14" s="8">
-        <v>157</v>
-      </c>
-      <c r="W14" s="8">
-        <v>166</v>
-      </c>
-      <c r="X14" s="8">
-        <v>167</v>
-      </c>
-      <c r="Y14" s="8">
-        <v>168</v>
-      </c>
-      <c r="Z14" s="8">
-        <v>169</v>
-      </c>
-      <c r="AA14" s="8">
-        <v>178</v>
-      </c>
-      <c r="AB14" s="8">
-        <v>179</v>
-      </c>
-      <c r="AC14" s="8">
-        <v>180</v>
-      </c>
-      <c r="AD14" s="8">
-        <v>181</v>
-      </c>
-      <c r="AE14" s="8">
-        <v>190</v>
-      </c>
-      <c r="AF14" s="8">
-        <v>191</v>
-      </c>
-      <c r="AG14" s="8">
-        <v>192</v>
-      </c>
-      <c r="AH14" s="8">
-        <v>193</v>
-      </c>
-      <c r="AI14" s="8">
-        <v>202</v>
-      </c>
-      <c r="AJ14" s="8">
-        <v>203</v>
-      </c>
-      <c r="AK14" s="8">
-        <v>204</v>
-      </c>
-      <c r="AL14" s="8">
-        <v>205</v>
-      </c>
-      <c r="AM14" s="8">
-        <v>214</v>
-      </c>
-      <c r="AN14" s="8">
-        <v>215</v>
-      </c>
-      <c r="AO14" s="8">
-        <v>216</v>
-      </c>
-      <c r="AP14" s="8">
-        <v>217</v>
-      </c>
-      <c r="AQ14" s="8">
-        <v>226</v>
-      </c>
-      <c r="AR14" s="8">
-        <v>227</v>
-      </c>
-      <c r="AS14" s="8">
-        <v>228</v>
-      </c>
-      <c r="AT14" s="8">
-        <v>229</v>
-      </c>
-      <c r="AU14" s="8">
-        <v>238</v>
-      </c>
-      <c r="AV14" s="8">
-        <v>239</v>
-      </c>
-      <c r="AW14" s="8">
-        <v>240</v>
-      </c>
-      <c r="AX14" s="8">
-        <v>241</v>
-      </c>
-      <c r="AY14" s="8">
-        <v>250</v>
-      </c>
-      <c r="AZ14" s="8">
-        <v>251</v>
-      </c>
-      <c r="BA14" s="8">
-        <v>252</v>
-      </c>
-      <c r="BB14" s="8">
-        <v>253</v>
-      </c>
-      <c r="BC14" s="8">
-        <v>262</v>
-      </c>
-      <c r="BD14" s="8">
-        <v>263</v>
-      </c>
-      <c r="BE14" s="8">
-        <v>264</v>
-      </c>
-      <c r="BF14" s="8">
-        <v>265</v>
-      </c>
-      <c r="BG14" s="8">
-        <v>274</v>
-      </c>
-      <c r="BH14" s="8">
-        <v>275</v>
-      </c>
-      <c r="BI14" s="8">
-        <v>276</v>
-      </c>
-      <c r="BJ14" s="8">
-        <v>277</v>
-      </c>
-      <c r="BK14" s="8">
-        <v>286</v>
-      </c>
-      <c r="BL14" s="8">
-        <v>287</v>
-      </c>
-      <c r="BM14" s="8">
-        <v>288</v>
-      </c>
-      <c r="BN14" s="8">
-        <v>289</v>
-      </c>
-      <c r="BO14" s="8">
-        <v>298</v>
-      </c>
-      <c r="BP14" s="8">
-        <v>299</v>
-      </c>
-      <c r="BQ14" s="8">
-        <v>300</v>
-      </c>
-      <c r="BR14" s="8">
-        <v>301</v>
-      </c>
-      <c r="BS14" s="8">
-        <v>310</v>
-      </c>
-      <c r="BT14" s="8">
-        <v>311</v>
-      </c>
-      <c r="BU14" s="8">
-        <v>312</v>
-      </c>
-      <c r="BV14" s="8">
-        <v>313</v>
-      </c>
-      <c r="BW14" s="8">
-        <v>314</v>
-      </c>
-      <c r="BX14" s="8">
-        <v>315</v>
-      </c>
-      <c r="BY14" s="8"/>
-      <c r="BZ14" s="8"/>
-      <c r="CA14" s="8"/>
-      <c r="CB14" s="8"/>
-      <c r="CC14" s="8"/>
-      <c r="CD14" s="8"/>
-      <c r="CE14" s="8"/>
-      <c r="CF14" s="8"/>
-      <c r="CG14" s="8"/>
-      <c r="CH14" s="8"/>
-      <c r="CI14" s="8"/>
-      <c r="CJ14" s="8"/>
-      <c r="CK14" s="8"/>
-      <c r="CL14" s="8"/>
-      <c r="CM14" s="8"/>
-      <c r="CN14" s="8"/>
-      <c r="CO14" s="8"/>
-      <c r="CP14" s="8"/>
-      <c r="CQ14" s="8"/>
-      <c r="CR14" s="8"/>
-      <c r="CS14" s="8"/>
-      <c r="CT14" s="8"/>
-      <c r="CU14" s="8"/>
-      <c r="CV14" s="8"/>
-      <c r="CW14" s="8"/>
-      <c r="CX14" s="8"/>
-      <c r="CY14" s="8"/>
-      <c r="CZ14" s="8"/>
-      <c r="DA14" s="8"/>
-      <c r="DB14" s="8"/>
-      <c r="DC14" s="8"/>
-      <c r="DD14" s="8"/>
-      <c r="DE14" s="8"/>
-      <c r="DF14" s="8"/>
-      <c r="DG14" s="8"/>
-      <c r="DH14" s="8"/>
-      <c r="DI14" s="8"/>
-      <c r="DJ14" s="8"/>
-      <c r="DK14" s="8"/>
-      <c r="DL14" s="8"/>
-      <c r="DM14" s="8"/>
-      <c r="DN14" s="8"/>
-      <c r="DO14" s="8"/>
-      <c r="DP14" s="8"/>
-      <c r="DQ14" s="8"/>
-      <c r="DR14" s="8"/>
-      <c r="DS14" s="8"/>
-      <c r="DT14" s="8"/>
-      <c r="DU14" s="8"/>
-      <c r="DV14" s="8"/>
-      <c r="DW14" s="8"/>
-      <c r="DX14" s="8"/>
-      <c r="DY14" s="8"/>
-      <c r="DZ14" s="8"/>
-      <c r="EA14" s="8"/>
-      <c r="EB14" s="8"/>
-    </row>
-    <row r="15" spans="1:132" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:132" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="B16" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B17" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B18" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B19" s="8">
         <v>16</v>
@@ -12631,38 +12112,18 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B20" s="8">
-        <v>8640</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B21" s="8">
         <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -12688,306 +12149,306 @@
   <sheetData>
     <row r="1" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C1" s="17">
         <v>3</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C2" s="17">
         <v>6</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C3" s="17">
         <v>16</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C4" s="17">
         <v>57</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C5" s="17">
         <v>50</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C6" s="18">
         <v>12</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C7" s="17">
         <v>6</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C8" s="17">
         <v>10</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C9" s="17">
         <v>20</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C10" s="17">
         <v>6.5</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C11" s="17">
         <v>2.7</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C12" s="17">
         <v>2</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C13" s="17">
         <v>8</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C18" s="17">
         <v>1000</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C19" s="17">
         <v>1</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C20" s="17">
         <v>1</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C21" s="17">
         <v>1</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C22" s="16">
         <v>0</v>
@@ -13021,72 +12482,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="A1" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="K2" s="23"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J3" t="s">
         <v>156</v>
       </c>
-      <c r="F3" t="s">
+      <c r="K3" t="s">
         <v>157</v>
-      </c>
-      <c r="G3" t="s">
-        <v>159</v>
-      </c>
-      <c r="H3" t="s">
-        <v>160</v>
-      </c>
-      <c r="I3" t="s">
-        <v>158</v>
-      </c>
-      <c r="J3" t="s">
-        <v>162</v>
-      </c>
-      <c r="K3" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -13234,29 +12695,29 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
+      <c r="A9" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Important Improvements and fixes to Canvas scaling
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8896FDF-B1DF-4560-BADF-138D2D906320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73375D68-D06F-4A2A-90D0-508E0BB2C379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="2" r:id="rId1"/>
     <sheet name="TrackVars" sheetId="3" r:id="rId2"/>
     <sheet name="TrackConstants" sheetId="4" r:id="rId3"/>
     <sheet name="PlotCorrelation" sheetId="5" r:id="rId4"/>
+    <sheet name="invertY" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="164">
   <si>
     <t>File</t>
   </si>
@@ -542,6 +543,15 @@
   </si>
   <si>
     <t>hm and mec regions defined in Platypus should follow the indexing in the y direction.</t>
+  </si>
+  <si>
+    <t>Factors at play</t>
+  </si>
+  <si>
+    <t>model.matrix row y position</t>
+  </si>
+  <si>
+    <t>model.matrix row index containing what region</t>
   </si>
 </sst>
 </file>
@@ -825,13 +835,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1058,10 +1068,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1900</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3600</c:v>
+                  <c:v>4300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1073,10 +1083,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1900</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3600</c:v>
+                  <c:v>4300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9350,50 +9360,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>8965</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>81951</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>35931</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3023CFA-79C1-46AE-B668-66A9AED7CAD8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3155577" y="11734800"/>
-          <a:ext cx="14631668" cy="5997460"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9623,6 +9589,114 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>157753</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>17793</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>21261</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE126A33-0CA6-4372-BDA5-CEB3B3A8A3B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2908573" y="0"/>
+          <a:ext cx="4736840" cy="569901"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9614249-D5D3-41BC-AF35-48D6DCBC64E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect r="3547" b="6422"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2903220" y="609600"/>
+          <a:ext cx="4754880" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -9940,8 +10014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10000,7 +10074,7 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G2" s="7" t="str">
-        <v>Node</v>
+        <v>checkSpatialMapping</v>
       </c>
       <c r="H2" s="7">
         <v>0</v>
@@ -10024,7 +10098,7 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G3" s="7" t="str">
-        <v>Region</v>
+        <v>setRegionIndices</v>
       </c>
       <c r="H3" s="7">
         <v>0</v>
@@ -10048,7 +10122,7 @@
         <v>LIM_Grid</v>
       </c>
       <c r="G4" s="7" t="str">
-        <v>meshBoundary</v>
+        <v>finalizeGrid</v>
       </c>
       <c r="H4" s="7">
         <v>0</v>
@@ -10069,10 +10143,10 @@
       </c>
       <c r="D5" s="2"/>
       <c r="F5" s="7" t="str">
-        <v>LIM_Grid</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G5" s="7" t="str">
-        <v>checkSpatialMapping</v>
+        <v>linalg_lu</v>
       </c>
       <c r="H5" s="7">
         <v>0</v>
@@ -10093,10 +10167,10 @@
       </c>
       <c r="D6" s="1"/>
       <c r="F6" s="7" t="str">
-        <v>LIM_Grid</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G6" s="7" t="str">
-        <v>buildGrid</v>
+        <v>dirichlet</v>
       </c>
       <c r="H6" s="7">
         <v>0</v>
@@ -10105,7 +10179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -10113,14 +10187,14 @@
         <v>14</v>
       </c>
       <c r="C7" s="14">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="7" t="str">
-        <v>LIM_Grid</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G7" s="7" t="str">
-        <v>setRegionIndices</v>
+        <v>hmHm</v>
       </c>
       <c r="H7" s="7">
         <v>0</v>
@@ -10137,14 +10211,14 @@
         <v>15</v>
       </c>
       <c r="C8" s="14">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="7" t="str">
-        <v>LIM_Grid</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G8" s="7" t="str">
-        <v>finalizeGrid</v>
+        <v>mecHm</v>
       </c>
       <c r="H8" s="7">
         <v>0</v>
@@ -10168,7 +10242,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G9" s="7" t="str">
-        <v>mecHm</v>
+        <v>mec</v>
       </c>
       <c r="H9" s="7">
         <v>0</v>
@@ -10177,7 +10251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -10185,14 +10259,14 @@
         <v>17</v>
       </c>
       <c r="C10" s="14">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D10" s="1"/>
       <c r="F10" s="7" t="str">
         <v>LIM_Compute</v>
       </c>
       <c r="G10" s="7" t="str">
-        <v>mec</v>
+        <v>preEqn24_2018</v>
       </c>
       <c r="H10" s="7">
         <v>0</v>
@@ -10216,7 +10290,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G11" s="7" t="str">
-        <v>preEqn24_2018</v>
+        <v>preEqn25_2018</v>
       </c>
       <c r="H11" s="7">
         <v>0</v>
@@ -10225,7 +10299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -10233,14 +10307,14 @@
         <v>46</v>
       </c>
       <c r="C12" s="14">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="7" t="str">
         <v>LIM_Compute</v>
       </c>
       <c r="G12" s="7" t="str">
-        <v>preEqn25_2018</v>
+        <v>preEqn8</v>
       </c>
       <c r="H12" s="7">
         <v>0</v>
@@ -10264,7 +10338,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G13" s="7" t="str">
-        <v>preEqn8</v>
+        <v>postEqn8</v>
       </c>
       <c r="H13" s="7">
         <v>0</v>
@@ -10288,7 +10362,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G14" s="7" t="str">
-        <v>postEqn8</v>
+        <v>postEqn9</v>
       </c>
       <c r="H14" s="7">
         <v>0</v>
@@ -10312,7 +10386,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G15" s="7" t="str">
-        <v>postEqn9</v>
+        <v>postEqn14to15</v>
       </c>
       <c r="H15" s="7">
         <v>0</v>
@@ -10329,14 +10403,14 @@
         <v>19</v>
       </c>
       <c r="C16" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D16" s="3"/>
       <c r="F16" s="7" t="str">
         <v>LIM_Compute</v>
       </c>
       <c r="G16" s="7" t="str">
-        <v>postEqn14to15</v>
+        <v>postEqn16to17</v>
       </c>
       <c r="H16" s="7">
         <v>0</v>
@@ -10353,14 +10427,14 @@
         <v>59</v>
       </c>
       <c r="C17" s="23">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D17" s="3"/>
       <c r="F17" s="7" t="str">
         <v>LIM_Compute</v>
       </c>
       <c r="G17" s="7" t="str">
-        <v>postEqn16to17</v>
+        <v>preEqn21</v>
       </c>
       <c r="H17" s="7">
         <v>0</v>
@@ -10377,14 +10451,14 @@
         <v>60</v>
       </c>
       <c r="C18" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D18" s="3"/>
       <c r="F18" s="7" t="str">
         <v>LIM_Compute</v>
       </c>
       <c r="G18" s="7" t="str">
-        <v>preEqn21</v>
+        <v>postEqn21</v>
       </c>
       <c r="H18" s="7">
         <v>0</v>
@@ -10408,7 +10482,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G19" s="7" t="str">
-        <v>postEqn21</v>
+        <v>eqn23Integral</v>
       </c>
       <c r="H19" s="7">
         <v>0</v>
@@ -10432,7 +10506,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G20" s="7" t="str">
-        <v>eqn23Integral</v>
+        <v>checkForErrors</v>
       </c>
       <c r="H20" s="7">
         <v>0</v>
@@ -10456,7 +10530,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G21" s="7" t="str">
-        <v>genForces</v>
+        <v>neighbourNodes</v>
       </c>
       <c r="H21" s="7">
         <v>0</v>
@@ -10480,7 +10554,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G22" s="7" t="str">
-        <v>plotPointsAlongX</v>
+        <v>boundaryInfo</v>
       </c>
       <c r="H22" s="7">
         <v>0</v>
@@ -10504,13 +10578,13 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G23" s="7" t="str">
-        <v>updateGrid</v>
+        <v>reduceMatrix</v>
       </c>
       <c r="H23" s="7">
         <v>0</v>
       </c>
-      <c r="I23" s="7" t="str">
-        <v>There are some errors with .phiError</v>
+      <c r="I23" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -10525,10 +10599,10 @@
       </c>
       <c r="D24" s="3"/>
       <c r="F24" s="7" t="str">
-        <v>LIM_Show</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G24" s="7" t="str">
-        <v>colorFader</v>
+        <v>buildMatAB</v>
       </c>
       <c r="H24" s="7">
         <v>0</v>
@@ -10549,10 +10623,10 @@
       </c>
       <c r="D25" s="3"/>
       <c r="F25" s="7" t="str">
-        <v>LIM_Show</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G25" s="7" t="str">
-        <v>myColourNumber</v>
+        <v>updateLists</v>
       </c>
       <c r="H25" s="7">
         <v>0</v>
@@ -10573,10 +10647,10 @@
       </c>
       <c r="D26" s="3"/>
       <c r="F26" s="7" t="str">
-        <v>LIM_Show</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G26" s="7" t="str">
-        <v>determineColour</v>
+        <v>shiftHmIdxList</v>
       </c>
       <c r="H26" s="7">
         <v>0</v>
@@ -10597,10 +10671,10 @@
       </c>
       <c r="D27" s="3"/>
       <c r="F27" s="7" t="str">
-        <v>LIM_Show</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G27" s="7" t="str">
-        <v>minMaxField</v>
+        <v>finalizeCompute</v>
       </c>
       <c r="H27" s="7">
         <v>0</v>
@@ -10621,10 +10695,10 @@
       </c>
       <c r="D28" s="3"/>
       <c r="F28" s="7" t="str">
-        <v>LIM_Show</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G28" s="7" t="str">
-        <v>combineFilterList</v>
+        <v>genForces</v>
       </c>
       <c r="H28" s="7">
         <v>0</v>
@@ -10645,10 +10719,10 @@
       </c>
       <c r="D29" s="3"/>
       <c r="F29" s="7" t="str">
-        <v>LIM_Show</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G29" s="7" t="str">
-        <v>genCanvasMatrix</v>
+        <v>plotPointsAlongX</v>
       </c>
       <c r="H29" s="7">
         <v>0</v>
@@ -10669,16 +10743,16 @@
       </c>
       <c r="D30" s="3"/>
       <c r="F30" s="7" t="str">
-        <v>LIM_Show</v>
+        <v>LIM_Compute</v>
       </c>
       <c r="G30" s="7" t="str">
-        <v>visualizeMatrix</v>
+        <v>updateGrid</v>
       </c>
       <c r="H30" s="7">
         <v>0</v>
       </c>
-      <c r="I30" s="7">
-        <v>0</v>
+      <c r="I30" s="7" t="str">
+        <v>There are some errors with .phiError</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -10696,7 +10770,7 @@
         <v>LIM_Show</v>
       </c>
       <c r="G31" s="7" t="str">
-        <v>showModel</v>
+        <v>colorFader</v>
       </c>
       <c r="H31" s="7">
         <v>0</v>
@@ -10713,14 +10787,14 @@
         <v>58</v>
       </c>
       <c r="C32" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D32" s="3"/>
       <c r="F32" s="7" t="str">
-        <v>LIM_ShowFromJSON</v>
+        <v>LIM_Show</v>
       </c>
       <c r="G32" s="7" t="str">
-        <v>plotPointsAlongX</v>
+        <v>myColourNumber</v>
       </c>
       <c r="H32" s="7">
         <v>0</v>
@@ -10737,14 +10811,14 @@
         <v>57</v>
       </c>
       <c r="C33" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D33" s="3"/>
       <c r="F33" s="7" t="str">
-        <v>LIM_ShowFromJSON</v>
+        <v>LIM_Show</v>
       </c>
       <c r="G33" s="7" t="str">
-        <v>main</v>
+        <v>determineColour</v>
       </c>
       <c r="H33" s="7">
         <v>0</v>
@@ -10761,14 +10835,14 @@
         <v>56</v>
       </c>
       <c r="C34" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D34" s="3"/>
       <c r="F34" s="7" t="str">
-        <v>Platypus</v>
+        <v>LIM_Show</v>
       </c>
       <c r="G34" s="7" t="str">
-        <v>destruct</v>
+        <v>minMaxField</v>
       </c>
       <c r="H34" s="7">
         <v>0</v>
@@ -10785,14 +10859,14 @@
         <v>30</v>
       </c>
       <c r="C35" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D35" s="3"/>
       <c r="F35" s="7" t="str">
-        <v>Platypus</v>
+        <v>LIM_Show</v>
       </c>
       <c r="G35" s="7" t="str">
-        <v>construct</v>
+        <v>combineFilterList</v>
       </c>
       <c r="H35" s="7">
         <v>0</v>
@@ -10809,14 +10883,14 @@
         <v>31</v>
       </c>
       <c r="C36" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D36" s="3"/>
       <c r="F36" s="7" t="str">
-        <v>Platypus</v>
+        <v>LIM_Show</v>
       </c>
       <c r="G36" s="7" t="str">
-        <v>jsonStoreSolution</v>
+        <v>genCanvasMatrix</v>
       </c>
       <c r="H36" s="7">
         <v>0</v>
@@ -10833,14 +10907,14 @@
         <v>55</v>
       </c>
       <c r="C37" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D37" s="3"/>
       <c r="F37" s="7" t="str">
-        <v>Platypus</v>
+        <v>LIM_Show</v>
       </c>
       <c r="G37" s="7" t="str">
-        <v>main</v>
+        <v>visualizeMatrix</v>
       </c>
       <c r="H37" s="7">
         <v>0</v>
@@ -10857,17 +10931,17 @@
         <v>54</v>
       </c>
       <c r="C38" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D38" s="3"/>
       <c r="F38" s="7" t="str">
-        <v>LIM_SlotPoleCalculation</v>
+        <v>LIM_Show</v>
       </c>
       <c r="G38" s="7" t="str">
-        <v>LimMotor</v>
+        <v>showModel</v>
       </c>
       <c r="H38" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I38" s="7">
         <v>0</v>
@@ -10881,17 +10955,17 @@
         <v>53</v>
       </c>
       <c r="C39" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D39" s="3"/>
       <c r="F39" s="7" t="str">
-        <v>LIM_SlotPoleCalculation</v>
+        <v>LIM_ShowFromJSON</v>
       </c>
       <c r="G39" s="7" t="str">
-        <v>Error</v>
+        <v>plotPointsAlongX</v>
       </c>
       <c r="H39" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I39" s="7">
         <v>0</v>
@@ -10909,13 +10983,13 @@
       </c>
       <c r="D40" s="3"/>
       <c r="F40" s="7" t="str">
-        <v>LIM_SlotPoleCalculation</v>
+        <v>LIM_ShowFromJSON</v>
       </c>
       <c r="G40" s="7" t="str">
-        <v>np_find_nearest</v>
+        <v>main</v>
       </c>
       <c r="H40" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I40" s="7">
         <v>0</v>
@@ -10933,13 +11007,13 @@
       </c>
       <c r="D41" s="3"/>
       <c r="F41" s="7" t="str">
-        <v>LIM_SlotPoleCalculation</v>
+        <v>Platypus</v>
       </c>
       <c r="G41" s="7" t="str">
-        <v>timing</v>
+        <v>destruct</v>
       </c>
       <c r="H41" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I41" s="7">
         <v>0</v>
@@ -10959,13 +11033,13 @@
         <v>157</v>
       </c>
       <c r="F42" s="7" t="str">
-        <v>LIM_Grid</v>
+        <v>Platypus</v>
       </c>
       <c r="G42" s="7" t="str">
-        <v>Grid</v>
+        <v>construct</v>
       </c>
       <c r="H42" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I42" s="7">
         <v>0</v>
@@ -10983,13 +11057,13 @@
       </c>
       <c r="D43" s="4"/>
       <c r="F43" s="7" t="str">
-        <v>LIM_Grid</v>
+        <v>Platypus</v>
       </c>
       <c r="G43" s="7" t="str">
-        <v>reluctance</v>
+        <v>jsonStoreSolution</v>
       </c>
       <c r="H43" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I43" s="7">
         <v>0</v>
@@ -11007,13 +11081,13 @@
       </c>
       <c r="D44" s="4"/>
       <c r="F44" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>Platypus</v>
       </c>
       <c r="G44" s="7" t="str">
-        <v>Model</v>
+        <v>main</v>
       </c>
       <c r="H44" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I44" s="7">
         <v>0</v>
@@ -11031,10 +11105,10 @@
       </c>
       <c r="D45" s="4"/>
       <c r="F45" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_SlotPoleCalculation</v>
       </c>
       <c r="G45" s="7" t="str">
-        <v>linalg_lu</v>
+        <v>LimMotor</v>
       </c>
       <c r="H45" s="7">
         <v>100</v>
@@ -11055,10 +11129,10 @@
       </c>
       <c r="D46" s="4"/>
       <c r="F46" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_SlotPoleCalculation</v>
       </c>
       <c r="G46" s="7" t="str">
-        <v>dirichlet</v>
+        <v>Error</v>
       </c>
       <c r="H46" s="7">
         <v>100</v>
@@ -11079,10 +11153,10 @@
       </c>
       <c r="D47" s="4"/>
       <c r="F47" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_SlotPoleCalculation</v>
       </c>
       <c r="G47" s="7" t="str">
-        <v>hmHm</v>
+        <v>np_find_nearest</v>
       </c>
       <c r="H47" s="7">
         <v>100</v>
@@ -11103,10 +11177,10 @@
       </c>
       <c r="D48" s="4"/>
       <c r="F48" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_SlotPoleCalculation</v>
       </c>
       <c r="G48" s="7" t="str">
-        <v>postMECAvgB</v>
+        <v>timing</v>
       </c>
       <c r="H48" s="7">
         <v>100</v>
@@ -11127,10 +11201,10 @@
       </c>
       <c r="D49" s="4"/>
       <c r="F49" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_Grid</v>
       </c>
       <c r="G49" s="7" t="str">
-        <v>checkForErrors</v>
+        <v>Grid</v>
       </c>
       <c r="H49" s="7">
         <v>100</v>
@@ -11151,10 +11225,10 @@
       </c>
       <c r="D50" s="4"/>
       <c r="F50" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_Grid</v>
       </c>
       <c r="G50" s="7" t="str">
-        <v>neighbourNodes</v>
+        <v>Node</v>
       </c>
       <c r="H50" s="7">
         <v>100</v>
@@ -11175,10 +11249,10 @@
       </c>
       <c r="D51" s="5"/>
       <c r="F51" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_Grid</v>
       </c>
       <c r="G51" s="7" t="str">
-        <v>boundaryInfo</v>
+        <v>Region</v>
       </c>
       <c r="H51" s="7">
         <v>100</v>
@@ -11199,10 +11273,10 @@
       </c>
       <c r="D52" s="5"/>
       <c r="F52" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_Grid</v>
       </c>
       <c r="G52" s="7" t="str">
-        <v>reduceMatrix</v>
+        <v>reluctance</v>
       </c>
       <c r="H52" s="7">
         <v>100</v>
@@ -11223,10 +11297,10 @@
       </c>
       <c r="D53" s="6"/>
       <c r="F53" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_Grid</v>
       </c>
       <c r="G53" s="7" t="str">
-        <v>buildMatAB</v>
+        <v>meshBoundary</v>
       </c>
       <c r="H53" s="7">
         <v>100</v>
@@ -11247,10 +11321,10 @@
       </c>
       <c r="D54" s="6"/>
       <c r="F54" s="7" t="str">
-        <v>LIM_Compute</v>
+        <v>LIM_Grid</v>
       </c>
       <c r="G54" s="7" t="str">
-        <v>updateLists</v>
+        <v>buildGrid</v>
       </c>
       <c r="H54" s="7">
         <v>100</v>
@@ -11274,7 +11348,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G55" s="7" t="str">
-        <v>shiftHmIdxList</v>
+        <v>Model</v>
       </c>
       <c r="H55" s="7">
         <v>100</v>
@@ -11298,7 +11372,7 @@
         <v>LIM_Compute</v>
       </c>
       <c r="G56" s="7" t="str">
-        <v>finalizeCompute</v>
+        <v>postMECAvgB</v>
       </c>
       <c r="H56" s="7">
         <v>100</v>
@@ -11313,11 +11387,11 @@
       </c>
       <c r="C57" s="7">
         <f>SUM(TrackIssues5[Confidence])</f>
-        <v>1900</v>
+        <v>1200</v>
       </c>
       <c r="D57" s="7">
         <f>ROWS(TrackIssues5[Confidence]) *100 - C57</f>
-        <v>3600</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -11348,12 +11422,12 @@
       <c r="C62" s="15"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="27" t="s">
+      <c r="A63" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="B63" s="27"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="20"/>
@@ -12466,38 +12540,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25" t="s">
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="K2" s="25"/>
+      <c r="K2" s="26"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -12679,29 +12753,29 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -12714,4 +12788,38 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E3EC59-2651-4706-B929-4FC0A25DD1E7}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working aigrap B plotting, still need to fix the thrust
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A5932C-E2B9-47D5-BE9D-9112E91D33D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31B9DE4-EBC0-4C7D-B8E9-88BD012686B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="169">
   <si>
     <t>File</t>
   </si>
@@ -542,9 +542,6 @@
     <t>Rules:</t>
   </si>
   <si>
-    <t>hm and mec regions defined in Platypus should follow the indexing in the y direction.</t>
-  </si>
-  <si>
     <t>Factors at play</t>
   </si>
   <si>
@@ -552,6 +549,24 @@
   </si>
   <si>
     <t>model.matrix row index containing what region</t>
+  </si>
+  <si>
+    <t>Things to do</t>
+  </si>
+  <si>
+    <t>continue looking through hmMec and mec methods</t>
+  </si>
+  <si>
+    <t>flip the regions (only use this to validate that the inversion regions are assigned correct). We want to continue without inversion</t>
+  </si>
+  <si>
+    <t>Pull up the old main buildMatAB method and compare to the current</t>
+  </si>
+  <si>
+    <t>We can remove the dirichlet indexes which would remove the need for removing an, bn and rows and allows me to match the paper better. Also in Show I can add some code that adds an offset to draw the vac regions</t>
+  </si>
+  <si>
+    <t>To get the Bx, By plots to match 2019 paper results; sim at pixelDiv = 10</t>
   </si>
 </sst>
 </file>
@@ -764,7 +779,7 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -833,6 +848,10 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -10014,8 +10033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11422,12 +11441,12 @@
       <c r="C62" s="15"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
+      <c r="A63" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="20"/>
@@ -12540,38 +12559,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="K2" s="26"/>
+      <c r="K2" s="28"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -12753,29 +12772,29 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -12792,34 +12811,60 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E3EC59-2651-4706-B929-4FC0A25DD1E7}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>161</v>
+      <c r="A1" s="25" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Now works for both mecOnly and HAM
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E862CEC-82B4-4416-B8B9-278EBA5CC92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F307DB-7AAD-4781-81A1-36507B5D58B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="165">
   <si>
     <t>File</t>
   </si>
@@ -552,6 +552,9 @@
   </si>
   <si>
     <t>&lt;-- Figure this out</t>
+  </si>
+  <si>
+    <t>GETTING MEC WORKING without hm is possible and described in 2015 paper. MEC is also more accurate for changing material like cores which means it can be used without hm. \</t>
   </si>
 </sst>
 </file>
@@ -2099,10 +2102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3563,9 +3566,42 @@
         <v>161</v>
       </c>
     </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="B72" s="26"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="26"/>
+      <c r="B73" s="26"/>
+      <c r="C73" s="26"/>
+      <c r="D73" s="26"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="26"/>
+      <c r="B74" s="26"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="26"/>
+      <c r="B75" s="26"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="26"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="26"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B63:E63"/>
+    <mergeCell ref="A72:D76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Clean up odd only airgap
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F307DB-7AAD-4781-81A1-36507B5D58B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E3CAE8-BF8D-431F-8E65-46EEBEDC4A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="2" r:id="rId1"/>
     <sheet name="TrackVars" sheetId="3" r:id="rId2"/>
-    <sheet name="TrackConstants" sheetId="4" r:id="rId3"/>
+    <sheet name="onlyMEC" sheetId="5" r:id="rId3"/>
+    <sheet name="TrackConstants" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="172">
   <si>
     <t>File</t>
   </si>
@@ -555,6 +556,27 @@
   </si>
   <si>
     <t>GETTING MEC WORKING without hm is possible and described in 2015 paper. MEC is also more accurate for changing material like cores which means it can be used without hm. \</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>We know that the HAM model was the correct magnitude in only the places that the BC has coils. The upper coil sections are not right and only had the right magnitude if MMF was multiplied by 100</t>
+  </si>
+  <si>
+    <t>This is backed up in onlyMEC where the entire B field in airgap was off by factor of 100. The crossover of the B field in airgap is also wrong. This shouldn't be too hard to debug because we are only using MEC</t>
+  </si>
+  <si>
+    <t>I think that the MMF is correct since we were getting the correct magnitude use HAM which uses the bottom MMF nodes</t>
+  </si>
+  <si>
+    <t>Go over all the pre-process math and post-process for anything that has to do with MEC and compare to paper</t>
+  </si>
+  <si>
+    <t>I have tried to validate pre and post process onlyMEC . I cannot get the waveform or magnitude to change, following the papers rules.</t>
+  </si>
+  <si>
+    <t>Look into other papers 2015 2018 and other for MEC theory</t>
   </si>
 </sst>
 </file>
@@ -2104,7 +2126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FE7BB8-5ABB-4E20-A918-8154C3182C64}">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A72" sqref="A72:D76"/>
     </sheetView>
   </sheetViews>
@@ -4344,6 +4366,56 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746B74A1-E2E9-411E-A31B-49675430CC3B}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470EA571-87DB-4BDA-819A-DD9B46927D19}">
   <dimension ref="A1:E22"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updates and Question - Optimizations
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E3CAE8-BF8D-431F-8E65-46EEBEDC4A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36328E2E-EA02-4703-87D7-24D14AA30009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
@@ -4370,7 +4370,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>